<commit_message>
update: Aggiornato file template con dati di test
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesho\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesho\Desktop\ore\ore-pws\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B83D575B-745E-4DF8-A52F-D084F0206E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5FA830-6EB7-4A8C-8930-BD7C6D76F81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1024,7 +1024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1035,21 +1035,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1070,20 +1060,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="13" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1101,19 +1077,6 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="13" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="13" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="13" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="13" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1137,31 +1100,19 @@
     <xf numFmtId="4" fontId="17" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="12" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="19" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="19" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="19" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="20" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="18" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="18" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="18" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="18" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="18" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1174,22 +1125,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="13" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1241,20 +1185,21 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="19" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="17" fontId="12" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -1266,17 +1211,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="12" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="19" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1285,8 +1234,6 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1301,36 +1248,82 @@
     <xf numFmtId="4" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="21" fillId="7" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="14" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="12" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="18" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="19" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="17" fontId="12" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1652,55 +1645,55 @@
       <pane xSplit="8" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" style="79" customWidth="1"/>
-    <col min="3" max="3" width="22" style="21" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" style="21" customWidth="1"/>
-    <col min="5" max="7" width="8.77734375" style="54" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" style="58" customWidth="1"/>
-    <col min="9" max="9" width="8.77734375" style="56" customWidth="1"/>
-    <col min="10" max="15" width="8.77734375" style="58" customWidth="1"/>
-    <col min="16" max="16" width="10.5546875" style="58" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" style="52" customWidth="1"/>
+    <col min="3" max="3" width="22" style="15" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" style="15" customWidth="1"/>
+    <col min="5" max="7" width="8.77734375" style="33" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" style="37" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" style="35" customWidth="1"/>
+    <col min="10" max="15" width="8.77734375" style="37" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" style="37" customWidth="1"/>
     <col min="17" max="17" width="5.44140625" customWidth="1"/>
-    <col min="18" max="18" width="6" style="85" customWidth="1"/>
-    <col min="19" max="19" width="7" style="73" customWidth="1"/>
-    <col min="20" max="20" width="8.109375" style="67" customWidth="1"/>
-    <col min="21" max="21" width="10.88671875" style="73" customWidth="1"/>
-    <col min="22" max="22" width="10.21875" style="73" customWidth="1"/>
+    <col min="18" max="18" width="6" style="56" customWidth="1"/>
+    <col min="19" max="19" width="7" style="48" customWidth="1"/>
+    <col min="20" max="20" width="8.109375" style="44" customWidth="1"/>
+    <col min="21" max="21" width="10.88671875" style="48" customWidth="1"/>
+    <col min="22" max="22" width="10.21875" style="48" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="125"/>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="143" t="s">
+      <c r="A1" s="96"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="131" t="s">
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
-      <c r="O1" s="126"/>
-      <c r="P1" s="126"/>
-      <c r="Q1" s="126"/>
-      <c r="R1" s="126"/>
-      <c r="S1" s="126"/>
-      <c r="T1" s="126"/>
-      <c r="U1" s="126"/>
-      <c r="V1" s="127"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="81"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
@@ -1713,72 +1706,72 @@
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
-      <c r="AI1" s="138"/>
-      <c r="AJ1" s="139"/>
-      <c r="AK1" s="139"/>
-      <c r="AL1" s="139"/>
-      <c r="AM1" s="139"/>
-      <c r="AN1" s="139"/>
-      <c r="AO1" s="139"/>
-      <c r="AP1" s="139"/>
-      <c r="AQ1" s="139"/>
-      <c r="AR1" s="139"/>
-      <c r="AS1" s="139"/>
-      <c r="AT1" s="139"/>
-      <c r="AU1" s="139"/>
-      <c r="AV1" s="139"/>
+      <c r="AI1" s="74"/>
+      <c r="AJ1" s="75"/>
+      <c r="AK1" s="75"/>
+      <c r="AL1" s="75"/>
+      <c r="AM1" s="75"/>
+      <c r="AN1" s="75"/>
+      <c r="AO1" s="75"/>
+      <c r="AP1" s="75"/>
+      <c r="AQ1" s="75"/>
+      <c r="AR1" s="75"/>
+      <c r="AS1" s="75"/>
+      <c r="AT1" s="75"/>
+      <c r="AU1" s="75"/>
+      <c r="AV1" s="75"/>
     </row>
     <row r="2" spans="1:48" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="114" t="s">
+      <c r="C2" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="114" t="s">
+      <c r="D2" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="134" t="s">
+      <c r="E2" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="145" t="s">
+      <c r="F2" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="134" t="s">
+      <c r="G2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="146" t="s">
+      <c r="H2" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="132" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="126"/>
-      <c r="L2" s="127"/>
-      <c r="M2" s="137" t="s">
+      <c r="K2" s="80"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="126"/>
-      <c r="O2" s="126"/>
-      <c r="P2" s="127"/>
-      <c r="Q2" s="117" t="s">
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="118"/>
-      <c r="S2" s="140" t="s">
+      <c r="R2" s="114"/>
+      <c r="S2" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="111" t="s">
+      <c r="T2" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="128" t="s">
+      <c r="U2" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="111" t="s">
+      <c r="V2" s="93" t="s">
         <v>15</v>
       </c>
       <c r="W2" s="2"/>
@@ -1793,58 +1786,58 @@
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
-      <c r="AI2" s="139"/>
-      <c r="AJ2" s="139"/>
-      <c r="AK2" s="139"/>
-      <c r="AL2" s="139"/>
-      <c r="AM2" s="139"/>
-      <c r="AN2" s="139"/>
-      <c r="AO2" s="139"/>
-      <c r="AP2" s="139"/>
-      <c r="AQ2" s="139"/>
-      <c r="AR2" s="139"/>
-      <c r="AS2" s="139"/>
-      <c r="AT2" s="139"/>
-      <c r="AU2" s="139"/>
-      <c r="AV2" s="139"/>
+      <c r="AI2" s="75"/>
+      <c r="AJ2" s="75"/>
+      <c r="AK2" s="75"/>
+      <c r="AL2" s="75"/>
+      <c r="AM2" s="75"/>
+      <c r="AN2" s="75"/>
+      <c r="AO2" s="75"/>
+      <c r="AP2" s="75"/>
+      <c r="AQ2" s="75"/>
+      <c r="AR2" s="75"/>
+      <c r="AS2" s="75"/>
+      <c r="AT2" s="75"/>
+      <c r="AU2" s="75"/>
+      <c r="AV2" s="75"/>
     </row>
     <row r="3" spans="1:48" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="107"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="121" t="s">
+      <c r="A3" s="112"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="115" t="s">
+      <c r="K3" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="109" t="s">
+      <c r="L3" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="121" t="s">
+      <c r="M3" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="115" t="s">
+      <c r="N3" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="109" t="s">
+      <c r="O3" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="133" t="s">
+      <c r="P3" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="119"/>
-      <c r="R3" s="120"/>
-      <c r="S3" s="141"/>
-      <c r="T3" s="112"/>
-      <c r="U3" s="129"/>
-      <c r="V3" s="112"/>
+      <c r="Q3" s="115"/>
+      <c r="R3" s="116"/>
+      <c r="S3" s="77"/>
+      <c r="T3" s="83"/>
+      <c r="U3" s="98"/>
+      <c r="V3" s="83"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
@@ -1857,48 +1850,48 @@
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
-      <c r="AI3" s="139"/>
-      <c r="AJ3" s="139"/>
-      <c r="AK3" s="139"/>
-      <c r="AL3" s="139"/>
-      <c r="AM3" s="139"/>
-      <c r="AN3" s="139"/>
-      <c r="AO3" s="139"/>
-      <c r="AP3" s="139"/>
-      <c r="AQ3" s="139"/>
-      <c r="AR3" s="139"/>
-      <c r="AS3" s="139"/>
-      <c r="AT3" s="139"/>
-      <c r="AU3" s="139"/>
-      <c r="AV3" s="139"/>
+      <c r="AI3" s="75"/>
+      <c r="AJ3" s="75"/>
+      <c r="AK3" s="75"/>
+      <c r="AL3" s="75"/>
+      <c r="AM3" s="75"/>
+      <c r="AN3" s="75"/>
+      <c r="AO3" s="75"/>
+      <c r="AP3" s="75"/>
+      <c r="AQ3" s="75"/>
+      <c r="AR3" s="75"/>
+      <c r="AS3" s="75"/>
+      <c r="AT3" s="75"/>
+      <c r="AU3" s="75"/>
+      <c r="AV3" s="75"/>
     </row>
     <row r="4" spans="1:48" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="108"/>
-      <c r="B4" s="113"/>
-      <c r="C4" s="113"/>
-      <c r="D4" s="113"/>
-      <c r="E4" s="113"/>
-      <c r="F4" s="113"/>
-      <c r="G4" s="113"/>
-      <c r="H4" s="113"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="108"/>
-      <c r="K4" s="116"/>
-      <c r="L4" s="110"/>
-      <c r="M4" s="108"/>
-      <c r="N4" s="116"/>
-      <c r="O4" s="110"/>
-      <c r="P4" s="113"/>
+      <c r="A4" s="106"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="106"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="84"/>
       <c r="Q4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="80" t="s">
+      <c r="R4" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="S4" s="142"/>
-      <c r="T4" s="113"/>
-      <c r="U4" s="130"/>
-      <c r="V4" s="113"/>
+      <c r="S4" s="78"/>
+      <c r="T4" s="84"/>
+      <c r="U4" s="99"/>
+      <c r="V4" s="84"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -1911,44 +1904,44 @@
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
-      <c r="AI4" s="139"/>
-      <c r="AJ4" s="139"/>
-      <c r="AK4" s="139"/>
-      <c r="AL4" s="139"/>
-      <c r="AM4" s="139"/>
-      <c r="AN4" s="139"/>
-      <c r="AO4" s="139"/>
-      <c r="AP4" s="139"/>
-      <c r="AQ4" s="139"/>
-      <c r="AR4" s="139"/>
-      <c r="AS4" s="139"/>
-      <c r="AT4" s="139"/>
-      <c r="AU4" s="139"/>
-      <c r="AV4" s="139"/>
+      <c r="AI4" s="75"/>
+      <c r="AJ4" s="75"/>
+      <c r="AK4" s="75"/>
+      <c r="AL4" s="75"/>
+      <c r="AM4" s="75"/>
+      <c r="AN4" s="75"/>
+      <c r="AO4" s="75"/>
+      <c r="AP4" s="75"/>
+      <c r="AQ4" s="75"/>
+      <c r="AR4" s="75"/>
+      <c r="AS4" s="75"/>
+      <c r="AT4" s="75"/>
+      <c r="AU4" s="75"/>
+      <c r="AV4" s="75"/>
     </row>
     <row r="5" spans="1:48" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="87"/>
-      <c r="B5" s="103"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="94"/>
-      <c r="L5" s="95"/>
-      <c r="M5" s="96"/>
-      <c r="N5" s="94"/>
-      <c r="O5" s="94"/>
-      <c r="P5" s="97"/>
-      <c r="Q5" s="98"/>
-      <c r="R5" s="99"/>
-      <c r="S5" s="100"/>
-      <c r="T5" s="101"/>
-      <c r="U5" s="102"/>
-      <c r="V5" s="101"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="68"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="70"/>
+      <c r="T5" s="71"/>
+      <c r="U5" s="72"/>
+      <c r="V5" s="71"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
@@ -1961,1045 +1954,1045 @@
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
-      <c r="AI5" s="139"/>
-      <c r="AJ5" s="139"/>
-      <c r="AK5" s="139"/>
-      <c r="AL5" s="139"/>
-      <c r="AM5" s="139"/>
-      <c r="AN5" s="139"/>
-      <c r="AO5" s="139"/>
-      <c r="AP5" s="139"/>
-      <c r="AQ5" s="139"/>
-      <c r="AR5" s="139"/>
-      <c r="AS5" s="139"/>
-      <c r="AT5" s="139"/>
-      <c r="AU5" s="139"/>
-      <c r="AV5" s="139"/>
-    </row>
-    <row r="6" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="68"/>
-      <c r="T6" s="62"/>
-      <c r="U6" s="68"/>
-      <c r="V6" s="68"/>
-      <c r="AI6" s="139"/>
-      <c r="AJ6" s="139"/>
-      <c r="AK6" s="139"/>
-      <c r="AL6" s="139"/>
-      <c r="AM6" s="139"/>
-      <c r="AN6" s="139"/>
-      <c r="AO6" s="139"/>
-      <c r="AP6" s="139"/>
-      <c r="AQ6" s="139"/>
-      <c r="AR6" s="139"/>
-      <c r="AS6" s="139"/>
-      <c r="AT6" s="139"/>
-      <c r="AU6" s="139"/>
-      <c r="AV6" s="139"/>
+      <c r="AI5" s="75"/>
+      <c r="AJ5" s="75"/>
+      <c r="AK5" s="75"/>
+      <c r="AL5" s="75"/>
+      <c r="AM5" s="75"/>
+      <c r="AN5" s="75"/>
+      <c r="AO5" s="75"/>
+      <c r="AP5" s="75"/>
+      <c r="AQ5" s="75"/>
+      <c r="AR5" s="75"/>
+      <c r="AS5" s="75"/>
+      <c r="AT5" s="75"/>
+      <c r="AU5" s="75"/>
+      <c r="AV5" s="75"/>
+    </row>
+    <row r="6" spans="1:48" s="11" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="117"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="125"/>
+      <c r="K6" s="126"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="128"/>
+      <c r="N6" s="126"/>
+      <c r="O6" s="126"/>
+      <c r="P6" s="127"/>
+      <c r="Q6" s="129"/>
+      <c r="R6" s="130"/>
+      <c r="S6" s="131"/>
+      <c r="T6" s="132"/>
+      <c r="U6" s="131"/>
+      <c r="V6" s="131"/>
+      <c r="AI6" s="75"/>
+      <c r="AJ6" s="75"/>
+      <c r="AK6" s="75"/>
+      <c r="AL6" s="75"/>
+      <c r="AM6" s="75"/>
+      <c r="AN6" s="75"/>
+      <c r="AO6" s="75"/>
+      <c r="AP6" s="75"/>
+      <c r="AQ6" s="75"/>
+      <c r="AR6" s="75"/>
+      <c r="AS6" s="75"/>
+      <c r="AT6" s="75"/>
+      <c r="AU6" s="75"/>
+      <c r="AV6" s="75"/>
     </row>
     <row r="7" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="7"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="82"/>
-      <c r="S7" s="69"/>
-      <c r="T7" s="63"/>
-      <c r="U7" s="69"/>
-      <c r="V7" s="69"/>
-      <c r="AI7" s="139"/>
-      <c r="AJ7" s="139"/>
-      <c r="AK7" s="139"/>
-      <c r="AL7" s="139"/>
-      <c r="AM7" s="139"/>
-      <c r="AN7" s="139"/>
-      <c r="AO7" s="139"/>
-      <c r="AP7" s="139"/>
-      <c r="AQ7" s="139"/>
-      <c r="AR7" s="139"/>
-      <c r="AS7" s="139"/>
-      <c r="AT7" s="139"/>
-      <c r="AU7" s="139"/>
-      <c r="AV7" s="139"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="54"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45"/>
+      <c r="AI7" s="75"/>
+      <c r="AJ7" s="75"/>
+      <c r="AK7" s="75"/>
+      <c r="AL7" s="75"/>
+      <c r="AM7" s="75"/>
+      <c r="AN7" s="75"/>
+      <c r="AO7" s="75"/>
+      <c r="AP7" s="75"/>
+      <c r="AQ7" s="75"/>
+      <c r="AR7" s="75"/>
+      <c r="AS7" s="75"/>
+      <c r="AT7" s="75"/>
+      <c r="AU7" s="75"/>
+      <c r="AV7" s="75"/>
     </row>
     <row r="8" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="7"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="82"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="63"/>
-      <c r="U8" s="69"/>
-      <c r="V8" s="69"/>
-      <c r="AI8" s="139"/>
-      <c r="AJ8" s="139"/>
-      <c r="AK8" s="139"/>
-      <c r="AL8" s="139"/>
-      <c r="AM8" s="139"/>
-      <c r="AN8" s="139"/>
-      <c r="AO8" s="139"/>
-      <c r="AP8" s="139"/>
-      <c r="AQ8" s="139"/>
-      <c r="AR8" s="139"/>
-      <c r="AS8" s="139"/>
-      <c r="AT8" s="139"/>
-      <c r="AU8" s="139"/>
-      <c r="AV8" s="139"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="45"/>
+      <c r="V8" s="45"/>
+      <c r="AI8" s="75"/>
+      <c r="AJ8" s="75"/>
+      <c r="AK8" s="75"/>
+      <c r="AL8" s="75"/>
+      <c r="AM8" s="75"/>
+      <c r="AN8" s="75"/>
+      <c r="AO8" s="75"/>
+      <c r="AP8" s="75"/>
+      <c r="AQ8" s="75"/>
+      <c r="AR8" s="75"/>
+      <c r="AS8" s="75"/>
+      <c r="AT8" s="75"/>
+      <c r="AU8" s="75"/>
+      <c r="AV8" s="75"/>
     </row>
     <row r="9" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="82"/>
-      <c r="S9" s="69"/>
-      <c r="T9" s="63"/>
-      <c r="U9" s="69"/>
-      <c r="V9" s="69"/>
-      <c r="AI9" s="139"/>
-      <c r="AJ9" s="139"/>
-      <c r="AK9" s="139"/>
-      <c r="AL9" s="139"/>
-      <c r="AM9" s="139"/>
-      <c r="AN9" s="139"/>
-      <c r="AO9" s="139"/>
-      <c r="AP9" s="139"/>
-      <c r="AQ9" s="139"/>
-      <c r="AR9" s="139"/>
-      <c r="AS9" s="139"/>
-      <c r="AT9" s="139"/>
-      <c r="AU9" s="139"/>
-      <c r="AV9" s="139"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="54"/>
+      <c r="S9" s="45"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="45"/>
+      <c r="V9" s="45"/>
+      <c r="AI9" s="75"/>
+      <c r="AJ9" s="75"/>
+      <c r="AK9" s="75"/>
+      <c r="AL9" s="75"/>
+      <c r="AM9" s="75"/>
+      <c r="AN9" s="75"/>
+      <c r="AO9" s="75"/>
+      <c r="AP9" s="75"/>
+      <c r="AQ9" s="75"/>
+      <c r="AR9" s="75"/>
+      <c r="AS9" s="75"/>
+      <c r="AT9" s="75"/>
+      <c r="AU9" s="75"/>
+      <c r="AV9" s="75"/>
     </row>
     <row r="10" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="7"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="82"/>
-      <c r="S10" s="69"/>
-      <c r="T10" s="63"/>
-      <c r="U10" s="69"/>
-      <c r="V10" s="69"/>
-      <c r="AI10" s="139"/>
-      <c r="AJ10" s="139"/>
-      <c r="AK10" s="139"/>
-      <c r="AL10" s="139"/>
-      <c r="AM10" s="139"/>
-      <c r="AN10" s="139"/>
-      <c r="AO10" s="139"/>
-      <c r="AP10" s="139"/>
-      <c r="AQ10" s="139"/>
-      <c r="AR10" s="139"/>
-      <c r="AS10" s="139"/>
-      <c r="AT10" s="139"/>
-      <c r="AU10" s="139"/>
-      <c r="AV10" s="139"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="45"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="45"/>
+      <c r="V10" s="45"/>
+      <c r="AI10" s="75"/>
+      <c r="AJ10" s="75"/>
+      <c r="AK10" s="75"/>
+      <c r="AL10" s="75"/>
+      <c r="AM10" s="75"/>
+      <c r="AN10" s="75"/>
+      <c r="AO10" s="75"/>
+      <c r="AP10" s="75"/>
+      <c r="AQ10" s="75"/>
+      <c r="AR10" s="75"/>
+      <c r="AS10" s="75"/>
+      <c r="AT10" s="75"/>
+      <c r="AU10" s="75"/>
+      <c r="AV10" s="75"/>
     </row>
     <row r="11" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="7"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="82"/>
-      <c r="S11" s="69"/>
-      <c r="T11" s="63"/>
-      <c r="U11" s="69"/>
-      <c r="V11" s="69"/>
-      <c r="AI11" s="139"/>
-      <c r="AJ11" s="139"/>
-      <c r="AK11" s="139"/>
-      <c r="AL11" s="139"/>
-      <c r="AM11" s="139"/>
-      <c r="AN11" s="139"/>
-      <c r="AO11" s="139"/>
-      <c r="AP11" s="139"/>
-      <c r="AQ11" s="139"/>
-      <c r="AR11" s="139"/>
-      <c r="AS11" s="139"/>
-      <c r="AT11" s="139"/>
-      <c r="AU11" s="139"/>
-      <c r="AV11" s="139"/>
-    </row>
-    <row r="12" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A12" s="4"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="83"/>
-      <c r="S12" s="70"/>
-      <c r="T12" s="64"/>
-      <c r="U12" s="70"/>
-      <c r="V12" s="70"/>
-      <c r="AJ12" s="12"/>
-      <c r="AK12" s="12"/>
-      <c r="AL12" s="12"/>
-      <c r="AM12" s="12"/>
-      <c r="AN12" s="12"/>
-      <c r="AO12" s="12"/>
-      <c r="AP12" s="12"/>
-      <c r="AQ12" s="12"/>
-      <c r="AR12" s="12"/>
-      <c r="AS12" s="12"/>
-      <c r="AT12" s="12"/>
-      <c r="AU12" s="12"/>
-      <c r="AV12" s="12"/>
-    </row>
-    <row r="13" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A13" s="4"/>
-      <c r="B13" s="76"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="47"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="83"/>
-      <c r="S13" s="70"/>
-      <c r="T13" s="64"/>
-      <c r="U13" s="70"/>
-      <c r="V13" s="70"/>
-      <c r="AJ13" s="13"/>
-      <c r="AK13" s="13"/>
-      <c r="AL13" s="13"/>
-      <c r="AM13" s="13"/>
-      <c r="AN13" s="13"/>
-      <c r="AO13" s="13"/>
-      <c r="AP13" s="13"/>
-      <c r="AQ13" s="13"/>
-      <c r="AR13" s="13"/>
-      <c r="AS13" s="13"/>
-      <c r="AT13" s="13"/>
-      <c r="AU13" s="13"/>
-      <c r="AV13" s="13"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="45"/>
+      <c r="V11" s="45"/>
+      <c r="AI11" s="75"/>
+      <c r="AJ11" s="75"/>
+      <c r="AK11" s="75"/>
+      <c r="AL11" s="75"/>
+      <c r="AM11" s="75"/>
+      <c r="AN11" s="75"/>
+      <c r="AO11" s="75"/>
+      <c r="AP11" s="75"/>
+      <c r="AQ11" s="75"/>
+      <c r="AR11" s="75"/>
+      <c r="AS11" s="75"/>
+      <c r="AT11" s="75"/>
+      <c r="AU11" s="75"/>
+      <c r="AV11" s="75"/>
+    </row>
+    <row r="12" spans="1:48" s="11" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A12" s="117"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="134"/>
+      <c r="G12" s="135"/>
+      <c r="H12" s="136"/>
+      <c r="I12" s="124"/>
+      <c r="J12" s="137"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="55"/>
+      <c r="S12" s="46"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="46"/>
+      <c r="V12" s="46"/>
+      <c r="AJ12" s="138"/>
+      <c r="AK12" s="138"/>
+      <c r="AL12" s="138"/>
+      <c r="AM12" s="138"/>
+      <c r="AN12" s="138"/>
+      <c r="AO12" s="138"/>
+      <c r="AP12" s="138"/>
+      <c r="AQ12" s="138"/>
+      <c r="AR12" s="138"/>
+      <c r="AS12" s="138"/>
+      <c r="AT12" s="138"/>
+      <c r="AU12" s="138"/>
+      <c r="AV12" s="138"/>
+    </row>
+    <row r="13" spans="1:48" s="11" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A13" s="117"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="133"/>
+      <c r="F13" s="134"/>
+      <c r="G13" s="135"/>
+      <c r="H13" s="136"/>
+      <c r="I13" s="124"/>
+      <c r="J13" s="137"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="55"/>
+      <c r="S13" s="46"/>
+      <c r="T13" s="42"/>
+      <c r="U13" s="46"/>
+      <c r="V13" s="46"/>
+      <c r="AJ13" s="139"/>
+      <c r="AK13" s="139"/>
+      <c r="AL13" s="139"/>
+      <c r="AM13" s="139"/>
+      <c r="AN13" s="139"/>
+      <c r="AO13" s="139"/>
+      <c r="AP13" s="139"/>
+      <c r="AQ13" s="139"/>
+      <c r="AR13" s="139"/>
+      <c r="AS13" s="139"/>
+      <c r="AT13" s="139"/>
+      <c r="AU13" s="139"/>
+      <c r="AV13" s="139"/>
     </row>
     <row r="14" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A14" s="7"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="82"/>
-      <c r="S14" s="69"/>
-      <c r="T14" s="63"/>
-      <c r="U14" s="69"/>
-      <c r="V14" s="69"/>
-      <c r="AJ14" s="13"/>
-      <c r="AK14" s="13"/>
-      <c r="AL14" s="13"/>
-      <c r="AM14" s="13"/>
-      <c r="AN14" s="13"/>
-      <c r="AO14" s="13"/>
-      <c r="AP14" s="13"/>
-      <c r="AQ14" s="13"/>
-      <c r="AR14" s="13"/>
-      <c r="AS14" s="13"/>
-      <c r="AT14" s="13"/>
-      <c r="AU14" s="13"/>
-      <c r="AV14" s="13"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="45"/>
+      <c r="V14" s="45"/>
+      <c r="AJ14" s="7"/>
+      <c r="AK14" s="7"/>
+      <c r="AL14" s="7"/>
+      <c r="AM14" s="7"/>
+      <c r="AN14" s="7"/>
+      <c r="AO14" s="7"/>
+      <c r="AP14" s="7"/>
+      <c r="AQ14" s="7"/>
+      <c r="AR14" s="7"/>
+      <c r="AS14" s="7"/>
+      <c r="AT14" s="7"/>
+      <c r="AU14" s="7"/>
+      <c r="AV14" s="7"/>
     </row>
     <row r="15" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="7"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="82"/>
-      <c r="S15" s="69"/>
-      <c r="T15" s="63"/>
-      <c r="U15" s="69"/>
-      <c r="V15" s="69"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="41"/>
+      <c r="U15" s="45"/>
+      <c r="V15" s="45"/>
     </row>
     <row r="16" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="7"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="82"/>
-      <c r="S16" s="69"/>
-      <c r="T16" s="63"/>
-      <c r="U16" s="69"/>
-      <c r="V16" s="69"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="54"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="41"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="45"/>
     </row>
     <row r="17" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="7"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="82"/>
-      <c r="S17" s="69"/>
-      <c r="T17" s="63"/>
-      <c r="U17" s="69"/>
-      <c r="V17" s="69"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="41"/>
+      <c r="U17" s="45"/>
+      <c r="V17" s="45"/>
     </row>
     <row r="18" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="7"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="38"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="82"/>
-      <c r="S18" s="69"/>
-      <c r="T18" s="63"/>
-      <c r="U18" s="69"/>
-      <c r="V18" s="69"/>
-    </row>
-    <row r="19" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="4"/>
-      <c r="B19" s="76"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="86"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="47"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="83"/>
-      <c r="S19" s="70"/>
-      <c r="T19" s="64"/>
-      <c r="U19" s="70"/>
-      <c r="V19" s="70"/>
-    </row>
-    <row r="20" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="4"/>
-      <c r="B20" s="76"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="86"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="46"/>
-      <c r="O20" s="46"/>
-      <c r="P20" s="47"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="83"/>
-      <c r="S20" s="70"/>
-      <c r="T20" s="64"/>
-      <c r="U20" s="70"/>
-      <c r="V20" s="70"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="45"/>
+      <c r="T18" s="41"/>
+      <c r="U18" s="45"/>
+      <c r="V18" s="45"/>
+    </row>
+    <row r="19" spans="1:48" s="11" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="117"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="134"/>
+      <c r="G19" s="135"/>
+      <c r="H19" s="136"/>
+      <c r="I19" s="124"/>
+      <c r="J19" s="137"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="55"/>
+      <c r="S19" s="46"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="46"/>
+      <c r="V19" s="46"/>
+    </row>
+    <row r="20" spans="1:48" s="11" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="117"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="134"/>
+      <c r="G20" s="135"/>
+      <c r="H20" s="136"/>
+      <c r="I20" s="124"/>
+      <c r="J20" s="137"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="55"/>
+      <c r="S20" s="46"/>
+      <c r="T20" s="42"/>
+      <c r="U20" s="46"/>
+      <c r="V20" s="46"/>
     </row>
     <row r="21" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="7"/>
-      <c r="B21" s="75"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="38"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="82"/>
-      <c r="S21" s="69"/>
-      <c r="T21" s="63"/>
-      <c r="U21" s="69"/>
-      <c r="V21" s="69"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="45"/>
+      <c r="T21" s="41"/>
+      <c r="U21" s="45"/>
+      <c r="V21" s="45"/>
     </row>
     <row r="22" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="7"/>
-      <c r="B22" s="75"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="38"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="82"/>
-      <c r="S22" s="69"/>
-      <c r="T22" s="63"/>
-      <c r="U22" s="69"/>
-      <c r="V22" s="69"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="45"/>
+      <c r="T22" s="41"/>
+      <c r="U22" s="45"/>
+      <c r="V22" s="45"/>
     </row>
     <row r="23" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="7"/>
-      <c r="B23" s="75"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="39"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="82"/>
-      <c r="S23" s="69"/>
-      <c r="T23" s="63"/>
-      <c r="U23" s="69"/>
-      <c r="V23" s="69"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="45"/>
+      <c r="T23" s="41"/>
+      <c r="U23" s="45"/>
+      <c r="V23" s="45"/>
     </row>
     <row r="24" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="7"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="82"/>
-      <c r="S24" s="69"/>
-      <c r="T24" s="63"/>
-      <c r="U24" s="69"/>
-      <c r="V24" s="69"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="45"/>
+      <c r="T24" s="41"/>
+      <c r="U24" s="45"/>
+      <c r="V24" s="45"/>
     </row>
     <row r="25" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="7"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="40"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="82"/>
-      <c r="S25" s="69"/>
-      <c r="T25" s="69"/>
-      <c r="U25" s="69"/>
-      <c r="V25" s="69"/>
-    </row>
-    <row r="26" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="4"/>
-      <c r="B26" s="76"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="86"/>
-      <c r="K26" s="46"/>
-      <c r="L26" s="47"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="46"/>
-      <c r="P26" s="47"/>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="83"/>
-      <c r="S26" s="70"/>
-      <c r="T26" s="64"/>
-      <c r="U26" s="70"/>
-      <c r="V26" s="70"/>
-    </row>
-    <row r="27" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="4"/>
-      <c r="B27" s="76"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="86"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="48"/>
-      <c r="N27" s="46"/>
-      <c r="O27" s="46"/>
-      <c r="P27" s="47"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="83"/>
-      <c r="S27" s="70"/>
-      <c r="T27" s="64"/>
-      <c r="U27" s="70"/>
-      <c r="V27" s="70"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="54"/>
+      <c r="S25" s="45"/>
+      <c r="T25" s="45"/>
+      <c r="U25" s="45"/>
+      <c r="V25" s="45"/>
+    </row>
+    <row r="26" spans="1:48" s="11" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="117"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="133"/>
+      <c r="F26" s="134"/>
+      <c r="G26" s="135"/>
+      <c r="H26" s="136"/>
+      <c r="I26" s="124"/>
+      <c r="J26" s="137"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="55"/>
+      <c r="S26" s="46"/>
+      <c r="T26" s="42"/>
+      <c r="U26" s="46"/>
+      <c r="V26" s="46"/>
+    </row>
+    <row r="27" spans="1:48" s="11" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="117"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="133"/>
+      <c r="F27" s="134"/>
+      <c r="G27" s="135"/>
+      <c r="H27" s="136"/>
+      <c r="I27" s="124"/>
+      <c r="J27" s="137"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="55"/>
+      <c r="S27" s="46"/>
+      <c r="T27" s="42"/>
+      <c r="U27" s="46"/>
+      <c r="V27" s="46"/>
     </row>
     <row r="28" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="7"/>
-      <c r="B28" s="75"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="38"/>
-      <c r="O28" s="38"/>
-      <c r="P28" s="39"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="82"/>
-      <c r="S28" s="69"/>
-      <c r="T28" s="63"/>
-      <c r="U28" s="69"/>
-      <c r="V28" s="69"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="25"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="54"/>
+      <c r="S28" s="45"/>
+      <c r="T28" s="41"/>
+      <c r="U28" s="45"/>
+      <c r="V28" s="45"/>
     </row>
     <row r="29" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="7"/>
-      <c r="B29" s="75"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="38"/>
-      <c r="O29" s="38"/>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="82"/>
-      <c r="S29" s="69"/>
-      <c r="T29" s="63"/>
-      <c r="U29" s="69"/>
-      <c r="V29" s="69"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="54"/>
+      <c r="S29" s="45"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="45"/>
+      <c r="V29" s="45"/>
     </row>
     <row r="30" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="7"/>
-      <c r="B30" s="75"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="40"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="38"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="82"/>
-      <c r="S30" s="69"/>
-      <c r="T30" s="63"/>
-      <c r="U30" s="69"/>
-      <c r="V30" s="69"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="25"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="54"/>
+      <c r="S30" s="45"/>
+      <c r="T30" s="41"/>
+      <c r="U30" s="45"/>
+      <c r="V30" s="45"/>
     </row>
     <row r="31" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="7"/>
-      <c r="B31" s="75"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="40"/>
-      <c r="N31" s="38"/>
-      <c r="O31" s="38"/>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="82"/>
-      <c r="S31" s="69"/>
-      <c r="T31" s="63"/>
-      <c r="U31" s="69"/>
-      <c r="V31" s="69"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="54"/>
+      <c r="S31" s="45"/>
+      <c r="T31" s="41"/>
+      <c r="U31" s="45"/>
+      <c r="V31" s="45"/>
     </row>
     <row r="32" spans="1:48" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="7"/>
-      <c r="B32" s="77"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="51"/>
-      <c r="N32" s="49"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="50"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="84"/>
-      <c r="S32" s="71"/>
-      <c r="T32" s="65"/>
-      <c r="U32" s="71"/>
-      <c r="V32" s="71"/>
-      <c r="W32" s="17"/>
-      <c r="X32" s="17"/>
-      <c r="Y32" s="17"/>
-      <c r="Z32" s="17"/>
-      <c r="AA32" s="17"/>
-      <c r="AB32" s="17"/>
-      <c r="AC32" s="17"/>
-      <c r="AD32" s="17"/>
-      <c r="AE32" s="17"/>
-      <c r="AF32" s="17"/>
-      <c r="AG32" s="17"/>
-      <c r="AH32" s="17"/>
-      <c r="AI32" s="17"/>
-      <c r="AJ32" s="17"/>
-      <c r="AK32" s="17"/>
-      <c r="AL32" s="17"/>
-      <c r="AM32" s="17"/>
-      <c r="AN32" s="17"/>
-      <c r="AO32" s="17"/>
-      <c r="AP32" s="17"/>
-      <c r="AQ32" s="17"/>
-      <c r="AR32" s="17"/>
-      <c r="AS32" s="17"/>
-      <c r="AT32" s="17"/>
-      <c r="AU32" s="17"/>
-      <c r="AV32" s="17"/>
-    </row>
-    <row r="33" spans="1:39" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="4"/>
-      <c r="B33" s="76"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="86"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="48"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
-      <c r="P33" s="47"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="83"/>
-      <c r="S33" s="70"/>
-      <c r="T33" s="64"/>
-      <c r="U33" s="70"/>
-      <c r="V33" s="70"/>
-    </row>
-    <row r="34" spans="1:39" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="4"/>
-      <c r="B34" s="76"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44"/>
-      <c r="H34" s="45"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="86"/>
-      <c r="K34" s="46"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="46"/>
-      <c r="O34" s="46"/>
-      <c r="P34" s="47"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="83"/>
-      <c r="S34" s="70"/>
-      <c r="T34" s="64"/>
-      <c r="U34" s="70"/>
-      <c r="V34" s="70"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="29"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="55"/>
+      <c r="S32" s="46"/>
+      <c r="T32" s="42"/>
+      <c r="U32" s="46"/>
+      <c r="V32" s="46"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11"/>
+      <c r="Y32" s="11"/>
+      <c r="Z32" s="11"/>
+      <c r="AA32" s="11"/>
+      <c r="AB32" s="11"/>
+      <c r="AC32" s="11"/>
+      <c r="AD32" s="11"/>
+      <c r="AE32" s="11"/>
+      <c r="AF32" s="11"/>
+      <c r="AG32" s="11"/>
+      <c r="AH32" s="11"/>
+      <c r="AI32" s="11"/>
+      <c r="AJ32" s="11"/>
+      <c r="AK32" s="11"/>
+      <c r="AL32" s="11"/>
+      <c r="AM32" s="11"/>
+      <c r="AN32" s="11"/>
+      <c r="AO32" s="11"/>
+      <c r="AP32" s="11"/>
+      <c r="AQ32" s="11"/>
+      <c r="AR32" s="11"/>
+      <c r="AS32" s="11"/>
+      <c r="AT32" s="11"/>
+      <c r="AU32" s="11"/>
+      <c r="AV32" s="11"/>
+    </row>
+    <row r="33" spans="1:39" s="11" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="117"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="133"/>
+      <c r="F33" s="134"/>
+      <c r="G33" s="135"/>
+      <c r="H33" s="136"/>
+      <c r="I33" s="124"/>
+      <c r="J33" s="137"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="29"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="55"/>
+      <c r="S33" s="46"/>
+      <c r="T33" s="42"/>
+      <c r="U33" s="46"/>
+      <c r="V33" s="46"/>
+    </row>
+    <row r="34" spans="1:39" s="11" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="117"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="133"/>
+      <c r="F34" s="134"/>
+      <c r="G34" s="135"/>
+      <c r="H34" s="136"/>
+      <c r="I34" s="124"/>
+      <c r="J34" s="137"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="29"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="55"/>
+      <c r="S34" s="46"/>
+      <c r="T34" s="42"/>
+      <c r="U34" s="46"/>
+      <c r="V34" s="46"/>
     </row>
     <row r="35" spans="1:39" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="7"/>
-      <c r="B35" s="75"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="40"/>
-      <c r="N35" s="38"/>
-      <c r="O35" s="38"/>
-      <c r="P35" s="39"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="82"/>
-      <c r="S35" s="69"/>
-      <c r="T35" s="63"/>
-      <c r="U35" s="69"/>
-      <c r="V35" s="69"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="26"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="54"/>
+      <c r="S35" s="45"/>
+      <c r="T35" s="41"/>
+      <c r="U35" s="45"/>
+      <c r="V35" s="45"/>
     </row>
     <row r="36" spans="1:39" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="7"/>
-      <c r="B36" s="78"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="38"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="40"/>
-      <c r="N36" s="38"/>
-      <c r="O36" s="38"/>
-      <c r="P36" s="39"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="82"/>
-      <c r="S36" s="69"/>
-      <c r="T36" s="63"/>
-      <c r="U36" s="69"/>
-      <c r="V36" s="69"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="26"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="25"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="54"/>
+      <c r="S36" s="45"/>
+      <c r="T36" s="41"/>
+      <c r="U36" s="45"/>
+      <c r="V36" s="45"/>
     </row>
     <row r="37" spans="1:39" ht="28.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="104" t="s">
+      <c r="A37" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="105"/>
-      <c r="C37" s="105"/>
-      <c r="D37" s="135">
+      <c r="B37" s="110"/>
+      <c r="C37" s="110"/>
+      <c r="D37" s="103">
         <f>H37+J37+K37+L37+M37+N37+O37+P37+S37+T37+U37+V37</f>
         <v>0</v>
       </c>
-      <c r="E37" s="52"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="59">
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="38">
         <f>SUM(H6:H36)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="60"/>
-      <c r="J37" s="61">
+      <c r="I37" s="39"/>
+      <c r="J37" s="40">
         <f t="shared" ref="J37:V37" si="0">SUM(J6:J36)</f>
         <v>0</v>
       </c>
-      <c r="K37" s="61">
+      <c r="K37" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L37" s="61">
+      <c r="L37" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M37" s="61">
+      <c r="M37" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N37" s="61">
+      <c r="N37" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O37" s="61">
+      <c r="O37" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P37" s="61">
+      <c r="P37" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q37" s="122">
+      <c r="Q37" s="108">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R37" s="122">
+      <c r="R37" s="108">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S37" s="66">
+      <c r="S37" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T37" s="66">
+      <c r="T37" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U37" s="66">
+      <c r="U37" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V37" s="66">
+      <c r="V37" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W37" s="19"/>
-      <c r="X37" s="19"/>
-      <c r="Y37" s="19"/>
-      <c r="Z37" s="19"/>
-      <c r="AA37" s="19"/>
-      <c r="AB37" s="19"/>
-      <c r="AC37" s="19"/>
-      <c r="AD37" s="19"/>
-      <c r="AE37" s="19"/>
-      <c r="AF37" s="19"/>
-      <c r="AG37" s="19"/>
-      <c r="AH37" s="19"/>
-      <c r="AI37" s="19"/>
-      <c r="AJ37" s="19"/>
-      <c r="AK37" s="19"/>
-      <c r="AL37" s="19"/>
-      <c r="AM37" s="19"/>
+      <c r="W37" s="13"/>
+      <c r="X37" s="13"/>
+      <c r="Y37" s="13"/>
+      <c r="Z37" s="13"/>
+      <c r="AA37" s="13"/>
+      <c r="AB37" s="13"/>
+      <c r="AC37" s="13"/>
+      <c r="AD37" s="13"/>
+      <c r="AE37" s="13"/>
+      <c r="AF37" s="13"/>
+      <c r="AG37" s="13"/>
+      <c r="AH37" s="13"/>
+      <c r="AI37" s="13"/>
+      <c r="AJ37" s="13"/>
+      <c r="AK37" s="13"/>
+      <c r="AL37" s="13"/>
+      <c r="AM37" s="13"/>
     </row>
     <row r="38" spans="1:39" ht="19.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="123" t="s">
+      <c r="A38" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="124"/>
-      <c r="C38" s="124"/>
-      <c r="D38" s="136"/>
-      <c r="H38" s="55" t="s">
+      <c r="B38" s="95"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="104"/>
+      <c r="H38" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="J38" s="57" t="s">
+      <c r="J38" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="K38" s="57" t="s">
+      <c r="K38" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L38" s="57" t="s">
+      <c r="L38" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="M38" s="57" t="s">
+      <c r="M38" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="N38" s="57" t="s">
+      <c r="N38" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="O38" s="57" t="s">
+      <c r="O38" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="P38" s="57" t="s">
+      <c r="P38" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="Q38" s="113"/>
-      <c r="R38" s="113"/>
-      <c r="S38" s="72" t="s">
+      <c r="Q38" s="84"/>
+      <c r="R38" s="84"/>
+      <c r="S38" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="T38" s="72" t="s">
+      <c r="T38" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="U38" s="72" t="s">
+      <c r="U38" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="V38" s="72" t="s">
+      <c r="V38" s="47" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3020,17 +3013,7 @@
     <filterColumn colId="46" showButton="0"/>
   </autoFilter>
   <mergeCells count="31">
-    <mergeCell ref="AI1:AV11"/>
-    <mergeCell ref="S2:S4"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="V2:V4"/>
+    <mergeCell ref="R37:R38"/>
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="U2:U4"/>
@@ -3047,10 +3030,20 @@
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="T2:T4"/>
     <mergeCell ref="C2:C4"/>
+    <mergeCell ref="AI1:AV11"/>
+    <mergeCell ref="S2:S4"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="V2:V4"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="Q2:R3"/>
     <mergeCell ref="M3:M4"/>
-    <mergeCell ref="R37:R38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17 B18 B19 B20 B21 B22 B23 B24 B25 B26 B27 B28 B29 B30 B31 B32 B33 B34 B35 B36 B37" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
fix: Rimosso RESET che colorava tutto di bianco
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesho\Desktop\ore\ore-pws\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889D66BB-FF17-4240-B649-9975EB3E87A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E2F059-845E-4CC7-8F21-95AD7EE23E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1016,6 +1016,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1026,6 +1028,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1046,18 +1051,26 @@
     <xf numFmtId="4" fontId="17" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="12" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="19" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="20" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="18" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="18" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1112,12 +1125,59 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="12" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="18" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="19" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1210,66 +1270,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="18" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="18" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1587,58 +1587,58 @@
   <dimension ref="A1:AV38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="8" ySplit="5" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="5" topLeftCell="I24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="22" style="7" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" style="7" customWidth="1"/>
-    <col min="5" max="7" width="8.77734375" style="12" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" style="16" customWidth="1"/>
-    <col min="9" max="9" width="8.77734375" style="14" customWidth="1"/>
-    <col min="10" max="15" width="8.77734375" style="16" customWidth="1"/>
-    <col min="16" max="16" width="10.5546875" style="16" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="22" style="9" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" style="9" customWidth="1"/>
+    <col min="5" max="7" width="8.77734375" style="17" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" style="21" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" style="19" customWidth="1"/>
+    <col min="10" max="15" width="8.77734375" style="21" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" style="21" customWidth="1"/>
     <col min="17" max="17" width="5.44140625" customWidth="1"/>
-    <col min="18" max="18" width="6" style="26" customWidth="1"/>
-    <col min="19" max="19" width="7" style="23" customWidth="1"/>
-    <col min="20" max="20" width="8.109375" style="21" customWidth="1"/>
-    <col min="21" max="21" width="10.88671875" style="23" customWidth="1"/>
-    <col min="22" max="22" width="10.21875" style="23" customWidth="1"/>
+    <col min="18" max="18" width="6" style="35" customWidth="1"/>
+    <col min="19" max="19" width="7" style="30" customWidth="1"/>
+    <col min="20" max="20" width="8.109375" style="27" customWidth="1"/>
+    <col min="21" max="21" width="10.88671875" style="30" customWidth="1"/>
+    <col min="22" max="22" width="10.21875" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="51"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="80" t="s">
+      <c r="A1" s="83"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="57" t="s">
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="53"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="85"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
@@ -1651,72 +1651,72 @@
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
-      <c r="AI1" s="75"/>
-      <c r="AJ1" s="76"/>
-      <c r="AK1" s="76"/>
-      <c r="AL1" s="76"/>
-      <c r="AM1" s="76"/>
-      <c r="AN1" s="76"/>
-      <c r="AO1" s="76"/>
-      <c r="AP1" s="76"/>
-      <c r="AQ1" s="76"/>
-      <c r="AR1" s="76"/>
-      <c r="AS1" s="76"/>
-      <c r="AT1" s="76"/>
-      <c r="AU1" s="76"/>
-      <c r="AV1" s="76"/>
+      <c r="AI1" s="107"/>
+      <c r="AJ1" s="108"/>
+      <c r="AK1" s="108"/>
+      <c r="AL1" s="108"/>
+      <c r="AM1" s="108"/>
+      <c r="AN1" s="108"/>
+      <c r="AO1" s="108"/>
+      <c r="AP1" s="108"/>
+      <c r="AQ1" s="108"/>
+      <c r="AR1" s="108"/>
+      <c r="AS1" s="108"/>
+      <c r="AT1" s="108"/>
+      <c r="AU1" s="108"/>
+      <c r="AV1" s="108"/>
     </row>
     <row r="2" spans="1:48" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="58" t="s">
+      <c r="I2" s="11"/>
+      <c r="J2" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="52"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="66" t="s">
+      <c r="K2" s="84"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="86" t="s">
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="87"/>
-      <c r="S2" s="77" t="s">
+      <c r="R2" s="119"/>
+      <c r="S2" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="73" t="s">
+      <c r="T2" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="54" t="s">
+      <c r="U2" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="73" t="s">
+      <c r="V2" s="105" t="s">
         <v>15</v>
       </c>
       <c r="W2" s="2"/>
@@ -1731,58 +1731,58 @@
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
-      <c r="AI2" s="76"/>
-      <c r="AJ2" s="76"/>
-      <c r="AK2" s="76"/>
-      <c r="AL2" s="76"/>
-      <c r="AM2" s="76"/>
-      <c r="AN2" s="76"/>
-      <c r="AO2" s="76"/>
-      <c r="AP2" s="76"/>
-      <c r="AQ2" s="76"/>
-      <c r="AR2" s="76"/>
-      <c r="AS2" s="76"/>
-      <c r="AT2" s="76"/>
-      <c r="AU2" s="76"/>
-      <c r="AV2" s="76"/>
+      <c r="AI2" s="108"/>
+      <c r="AJ2" s="108"/>
+      <c r="AK2" s="108"/>
+      <c r="AL2" s="108"/>
+      <c r="AM2" s="108"/>
+      <c r="AN2" s="108"/>
+      <c r="AO2" s="108"/>
+      <c r="AP2" s="108"/>
+      <c r="AQ2" s="108"/>
+      <c r="AR2" s="108"/>
+      <c r="AS2" s="108"/>
+      <c r="AT2" s="108"/>
+      <c r="AU2" s="108"/>
+      <c r="AV2" s="108"/>
     </row>
     <row r="3" spans="1:48" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="70"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="64" t="s">
+      <c r="A3" s="102"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="82" t="s">
+      <c r="K3" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="64" t="s">
+      <c r="M3" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="82" t="s">
+      <c r="N3" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="59" t="s">
+      <c r="P3" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="88"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="78"/>
-      <c r="T3" s="61"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="61"/>
+      <c r="Q3" s="120"/>
+      <c r="R3" s="121"/>
+      <c r="S3" s="110"/>
+      <c r="T3" s="93"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="93"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
@@ -1795,48 +1795,48 @@
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
-      <c r="AI3" s="76"/>
-      <c r="AJ3" s="76"/>
-      <c r="AK3" s="76"/>
-      <c r="AL3" s="76"/>
-      <c r="AM3" s="76"/>
-      <c r="AN3" s="76"/>
-      <c r="AO3" s="76"/>
-      <c r="AP3" s="76"/>
-      <c r="AQ3" s="76"/>
-      <c r="AR3" s="76"/>
-      <c r="AS3" s="76"/>
-      <c r="AT3" s="76"/>
-      <c r="AU3" s="76"/>
-      <c r="AV3" s="76"/>
+      <c r="AI3" s="108"/>
+      <c r="AJ3" s="108"/>
+      <c r="AK3" s="108"/>
+      <c r="AL3" s="108"/>
+      <c r="AM3" s="108"/>
+      <c r="AN3" s="108"/>
+      <c r="AO3" s="108"/>
+      <c r="AP3" s="108"/>
+      <c r="AQ3" s="108"/>
+      <c r="AR3" s="108"/>
+      <c r="AS3" s="108"/>
+      <c r="AT3" s="108"/>
+      <c r="AU3" s="108"/>
+      <c r="AV3" s="108"/>
     </row>
     <row r="4" spans="1:48" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="65"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="48"/>
+      <c r="A4" s="97"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="115"/>
+      <c r="L4" s="104"/>
+      <c r="M4" s="97"/>
+      <c r="N4" s="115"/>
+      <c r="O4" s="104"/>
+      <c r="P4" s="80"/>
       <c r="Q4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="25" t="s">
+      <c r="R4" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="S4" s="79"/>
-      <c r="T4" s="48"/>
-      <c r="U4" s="56"/>
-      <c r="V4" s="48"/>
+      <c r="S4" s="111"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="80"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -1849,44 +1849,44 @@
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
-      <c r="AI4" s="76"/>
-      <c r="AJ4" s="76"/>
-      <c r="AK4" s="76"/>
-      <c r="AL4" s="76"/>
-      <c r="AM4" s="76"/>
-      <c r="AN4" s="76"/>
-      <c r="AO4" s="76"/>
-      <c r="AP4" s="76"/>
-      <c r="AQ4" s="76"/>
-      <c r="AR4" s="76"/>
-      <c r="AS4" s="76"/>
-      <c r="AT4" s="76"/>
-      <c r="AU4" s="76"/>
-      <c r="AV4" s="76"/>
+      <c r="AI4" s="108"/>
+      <c r="AJ4" s="108"/>
+      <c r="AK4" s="108"/>
+      <c r="AL4" s="108"/>
+      <c r="AM4" s="108"/>
+      <c r="AN4" s="108"/>
+      <c r="AO4" s="108"/>
+      <c r="AP4" s="108"/>
+      <c r="AQ4" s="108"/>
+      <c r="AR4" s="108"/>
+      <c r="AS4" s="108"/>
+      <c r="AT4" s="108"/>
+      <c r="AU4" s="108"/>
+      <c r="AV4" s="108"/>
     </row>
     <row r="5" spans="1:48" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="27"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="42"/>
-      <c r="V5" s="41"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="50"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="50"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
@@ -1899,1020 +1899,1020 @@
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
-      <c r="AI5" s="76"/>
-      <c r="AJ5" s="76"/>
-      <c r="AK5" s="76"/>
-      <c r="AL5" s="76"/>
-      <c r="AM5" s="76"/>
-      <c r="AN5" s="76"/>
-      <c r="AO5" s="76"/>
-      <c r="AP5" s="76"/>
-      <c r="AQ5" s="76"/>
-      <c r="AR5" s="76"/>
-      <c r="AS5" s="76"/>
-      <c r="AT5" s="76"/>
-      <c r="AU5" s="76"/>
-      <c r="AV5" s="76"/>
-    </row>
-    <row r="6" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="90"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="94"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="97"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="101"/>
-      <c r="N6" s="99"/>
-      <c r="O6" s="99"/>
-      <c r="P6" s="100"/>
-      <c r="Q6" s="102"/>
-      <c r="R6" s="103"/>
-      <c r="S6" s="104"/>
-      <c r="T6" s="105"/>
-      <c r="U6" s="104"/>
-      <c r="V6" s="104"/>
-      <c r="AI6" s="76"/>
-      <c r="AJ6" s="76"/>
-      <c r="AK6" s="76"/>
-      <c r="AL6" s="76"/>
-      <c r="AM6" s="76"/>
-      <c r="AN6" s="76"/>
-      <c r="AO6" s="76"/>
-      <c r="AP6" s="76"/>
-      <c r="AQ6" s="76"/>
-      <c r="AR6" s="76"/>
-      <c r="AS6" s="76"/>
-      <c r="AT6" s="76"/>
-      <c r="AU6" s="76"/>
-      <c r="AV6" s="76"/>
-    </row>
-    <row r="7" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="90"/>
-      <c r="B7" s="106"/>
-      <c r="C7" s="107"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="97"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="113"/>
-      <c r="M7" s="114"/>
-      <c r="N7" s="112"/>
-      <c r="O7" s="112"/>
-      <c r="P7" s="113"/>
-      <c r="Q7" s="115"/>
-      <c r="R7" s="116"/>
-      <c r="S7" s="117"/>
-      <c r="T7" s="118"/>
-      <c r="U7" s="117"/>
-      <c r="V7" s="117"/>
-      <c r="AI7" s="76"/>
-      <c r="AJ7" s="76"/>
-      <c r="AK7" s="76"/>
-      <c r="AL7" s="76"/>
-      <c r="AM7" s="76"/>
-      <c r="AN7" s="76"/>
-      <c r="AO7" s="76"/>
-      <c r="AP7" s="76"/>
-      <c r="AQ7" s="76"/>
-      <c r="AR7" s="76"/>
-      <c r="AS7" s="76"/>
-      <c r="AT7" s="76"/>
-      <c r="AU7" s="76"/>
-      <c r="AV7" s="76"/>
-    </row>
-    <row r="8" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="90"/>
-      <c r="B8" s="106"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="108"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="110"/>
-      <c r="I8" s="97"/>
-      <c r="J8" s="111"/>
-      <c r="K8" s="112"/>
-      <c r="L8" s="113"/>
-      <c r="M8" s="114"/>
-      <c r="N8" s="112"/>
-      <c r="O8" s="112"/>
-      <c r="P8" s="113"/>
-      <c r="Q8" s="115"/>
-      <c r="R8" s="116"/>
-      <c r="S8" s="117"/>
-      <c r="T8" s="118"/>
-      <c r="U8" s="117"/>
-      <c r="V8" s="117"/>
-      <c r="AI8" s="76"/>
-      <c r="AJ8" s="76"/>
-      <c r="AK8" s="76"/>
-      <c r="AL8" s="76"/>
-      <c r="AM8" s="76"/>
-      <c r="AN8" s="76"/>
-      <c r="AO8" s="76"/>
-      <c r="AP8" s="76"/>
-      <c r="AQ8" s="76"/>
-      <c r="AR8" s="76"/>
-      <c r="AS8" s="76"/>
-      <c r="AT8" s="76"/>
-      <c r="AU8" s="76"/>
-      <c r="AV8" s="76"/>
-    </row>
-    <row r="9" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="90"/>
-      <c r="B9" s="106"/>
-      <c r="C9" s="107"/>
-      <c r="D9" s="107"/>
-      <c r="E9" s="119"/>
-      <c r="F9" s="108"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="97"/>
-      <c r="J9" s="111"/>
-      <c r="K9" s="112"/>
-      <c r="L9" s="113"/>
-      <c r="M9" s="114"/>
-      <c r="N9" s="112"/>
-      <c r="O9" s="112"/>
-      <c r="P9" s="113"/>
-      <c r="Q9" s="115"/>
-      <c r="R9" s="116"/>
-      <c r="S9" s="117"/>
-      <c r="T9" s="118"/>
-      <c r="U9" s="117"/>
-      <c r="V9" s="117"/>
-      <c r="AI9" s="76"/>
-      <c r="AJ9" s="76"/>
-      <c r="AK9" s="76"/>
-      <c r="AL9" s="76"/>
-      <c r="AM9" s="76"/>
-      <c r="AN9" s="76"/>
-      <c r="AO9" s="76"/>
-      <c r="AP9" s="76"/>
-      <c r="AQ9" s="76"/>
-      <c r="AR9" s="76"/>
-      <c r="AS9" s="76"/>
-      <c r="AT9" s="76"/>
-      <c r="AU9" s="76"/>
-      <c r="AV9" s="76"/>
-    </row>
-    <row r="10" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="90"/>
-      <c r="B10" s="106"/>
-      <c r="C10" s="107"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="119"/>
-      <c r="F10" s="108"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="110"/>
-      <c r="I10" s="97"/>
-      <c r="J10" s="111"/>
-      <c r="K10" s="112"/>
-      <c r="L10" s="113"/>
-      <c r="M10" s="114"/>
-      <c r="N10" s="112"/>
-      <c r="O10" s="112"/>
-      <c r="P10" s="113"/>
-      <c r="Q10" s="115"/>
-      <c r="R10" s="116"/>
-      <c r="S10" s="117"/>
-      <c r="T10" s="118"/>
-      <c r="U10" s="117"/>
-      <c r="V10" s="117"/>
-      <c r="AI10" s="76"/>
-      <c r="AJ10" s="76"/>
-      <c r="AK10" s="76"/>
-      <c r="AL10" s="76"/>
-      <c r="AM10" s="76"/>
-      <c r="AN10" s="76"/>
-      <c r="AO10" s="76"/>
-      <c r="AP10" s="76"/>
-      <c r="AQ10" s="76"/>
-      <c r="AR10" s="76"/>
-      <c r="AS10" s="76"/>
-      <c r="AT10" s="76"/>
-      <c r="AU10" s="76"/>
-      <c r="AV10" s="76"/>
-    </row>
-    <row r="11" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="90"/>
-      <c r="B11" s="106"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="108"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="97"/>
-      <c r="J11" s="111"/>
-      <c r="K11" s="112"/>
-      <c r="L11" s="113"/>
-      <c r="M11" s="114"/>
-      <c r="N11" s="112"/>
-      <c r="O11" s="112"/>
-      <c r="P11" s="113"/>
-      <c r="Q11" s="115"/>
-      <c r="R11" s="116"/>
-      <c r="S11" s="117"/>
-      <c r="T11" s="118"/>
-      <c r="U11" s="117"/>
-      <c r="V11" s="117"/>
-      <c r="AI11" s="76"/>
-      <c r="AJ11" s="76"/>
-      <c r="AK11" s="76"/>
-      <c r="AL11" s="76"/>
-      <c r="AM11" s="76"/>
-      <c r="AN11" s="76"/>
-      <c r="AO11" s="76"/>
-      <c r="AP11" s="76"/>
-      <c r="AQ11" s="76"/>
-      <c r="AR11" s="76"/>
-      <c r="AS11" s="76"/>
-      <c r="AT11" s="76"/>
-      <c r="AU11" s="76"/>
-      <c r="AV11" s="76"/>
-    </row>
-    <row r="12" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A12" s="90"/>
-      <c r="B12" s="106"/>
-      <c r="C12" s="107"/>
-      <c r="D12" s="107"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="108"/>
-      <c r="G12" s="109"/>
-      <c r="H12" s="110"/>
-      <c r="I12" s="97"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="112"/>
-      <c r="L12" s="113"/>
-      <c r="M12" s="114"/>
-      <c r="N12" s="112"/>
-      <c r="O12" s="112"/>
-      <c r="P12" s="113"/>
-      <c r="Q12" s="115"/>
-      <c r="R12" s="116"/>
-      <c r="S12" s="117"/>
-      <c r="T12" s="118"/>
-      <c r="U12" s="117"/>
-      <c r="V12" s="117"/>
-      <c r="AJ12" s="44"/>
-      <c r="AK12" s="44"/>
-      <c r="AL12" s="44"/>
-      <c r="AM12" s="44"/>
-      <c r="AN12" s="44"/>
-      <c r="AO12" s="44"/>
-      <c r="AP12" s="44"/>
-      <c r="AQ12" s="44"/>
-      <c r="AR12" s="44"/>
-      <c r="AS12" s="44"/>
-      <c r="AT12" s="44"/>
-      <c r="AU12" s="44"/>
-      <c r="AV12" s="44"/>
-    </row>
-    <row r="13" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A13" s="90"/>
-      <c r="B13" s="106"/>
-      <c r="C13" s="107"/>
-      <c r="D13" s="107"/>
-      <c r="E13" s="119"/>
-      <c r="F13" s="108"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="110"/>
-      <c r="I13" s="97"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="112"/>
-      <c r="L13" s="113"/>
-      <c r="M13" s="114"/>
-      <c r="N13" s="112"/>
-      <c r="O13" s="112"/>
-      <c r="P13" s="113"/>
-      <c r="Q13" s="115"/>
-      <c r="R13" s="116"/>
-      <c r="S13" s="117"/>
-      <c r="T13" s="118"/>
-      <c r="U13" s="117"/>
-      <c r="V13" s="117"/>
-      <c r="AJ13" s="45"/>
-      <c r="AK13" s="45"/>
-      <c r="AL13" s="45"/>
-      <c r="AM13" s="45"/>
-      <c r="AN13" s="45"/>
-      <c r="AO13" s="45"/>
-      <c r="AP13" s="45"/>
-      <c r="AQ13" s="45"/>
-      <c r="AR13" s="45"/>
-      <c r="AS13" s="45"/>
-      <c r="AT13" s="45"/>
-      <c r="AU13" s="45"/>
-      <c r="AV13" s="45"/>
-    </row>
-    <row r="14" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A14" s="90"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="107"/>
-      <c r="E14" s="119"/>
-      <c r="F14" s="108"/>
-      <c r="G14" s="109"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="97"/>
-      <c r="J14" s="111"/>
-      <c r="K14" s="112"/>
-      <c r="L14" s="113"/>
-      <c r="M14" s="114"/>
-      <c r="N14" s="112"/>
-      <c r="O14" s="112"/>
-      <c r="P14" s="113"/>
-      <c r="Q14" s="115"/>
-      <c r="R14" s="116"/>
-      <c r="S14" s="117"/>
-      <c r="T14" s="118"/>
-      <c r="U14" s="117"/>
-      <c r="V14" s="117"/>
-      <c r="AJ14" s="45"/>
-      <c r="AK14" s="45"/>
-      <c r="AL14" s="45"/>
-      <c r="AM14" s="45"/>
-      <c r="AN14" s="45"/>
-      <c r="AO14" s="45"/>
-      <c r="AP14" s="45"/>
-      <c r="AQ14" s="45"/>
-      <c r="AR14" s="45"/>
-      <c r="AS14" s="45"/>
-      <c r="AT14" s="45"/>
-      <c r="AU14" s="45"/>
-      <c r="AV14" s="45"/>
-    </row>
-    <row r="15" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="90"/>
-      <c r="B15" s="106"/>
-      <c r="C15" s="107"/>
-      <c r="D15" s="107"/>
-      <c r="E15" s="119"/>
-      <c r="F15" s="108"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="110"/>
-      <c r="I15" s="97"/>
-      <c r="J15" s="111"/>
-      <c r="K15" s="112"/>
-      <c r="L15" s="113"/>
-      <c r="M15" s="114"/>
-      <c r="N15" s="112"/>
-      <c r="O15" s="112"/>
-      <c r="P15" s="113"/>
-      <c r="Q15" s="115"/>
-      <c r="R15" s="116"/>
-      <c r="S15" s="117"/>
-      <c r="T15" s="118"/>
-      <c r="U15" s="117"/>
-      <c r="V15" s="117"/>
-    </row>
-    <row r="16" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="90"/>
-      <c r="B16" s="106"/>
-      <c r="C16" s="107"/>
-      <c r="D16" s="107"/>
-      <c r="E16" s="119"/>
-      <c r="F16" s="108"/>
-      <c r="G16" s="109"/>
-      <c r="H16" s="110"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="111"/>
-      <c r="K16" s="112"/>
-      <c r="L16" s="113"/>
-      <c r="M16" s="114"/>
-      <c r="N16" s="112"/>
-      <c r="O16" s="112"/>
-      <c r="P16" s="113"/>
-      <c r="Q16" s="115"/>
-      <c r="R16" s="116"/>
-      <c r="S16" s="117"/>
-      <c r="T16" s="118"/>
-      <c r="U16" s="117"/>
-      <c r="V16" s="117"/>
-    </row>
-    <row r="17" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="90"/>
-      <c r="B17" s="106"/>
-      <c r="C17" s="107"/>
-      <c r="D17" s="107"/>
-      <c r="E17" s="119"/>
-      <c r="F17" s="108"/>
-      <c r="G17" s="109"/>
-      <c r="H17" s="110"/>
-      <c r="I17" s="97"/>
-      <c r="J17" s="111"/>
-      <c r="K17" s="112"/>
-      <c r="L17" s="113"/>
-      <c r="M17" s="114"/>
-      <c r="N17" s="112"/>
-      <c r="O17" s="112"/>
-      <c r="P17" s="113"/>
-      <c r="Q17" s="115"/>
-      <c r="R17" s="116"/>
-      <c r="S17" s="117"/>
-      <c r="T17" s="118"/>
-      <c r="U17" s="117"/>
-      <c r="V17" s="117"/>
-    </row>
-    <row r="18" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="90"/>
-      <c r="B18" s="106"/>
-      <c r="C18" s="107"/>
-      <c r="D18" s="107"/>
-      <c r="E18" s="119"/>
-      <c r="F18" s="108"/>
-      <c r="G18" s="109"/>
-      <c r="H18" s="110"/>
-      <c r="I18" s="97"/>
-      <c r="J18" s="111"/>
-      <c r="K18" s="112"/>
-      <c r="L18" s="113"/>
-      <c r="M18" s="114"/>
-      <c r="N18" s="112"/>
-      <c r="O18" s="112"/>
-      <c r="P18" s="113"/>
-      <c r="Q18" s="115"/>
-      <c r="R18" s="116"/>
-      <c r="S18" s="117"/>
-      <c r="T18" s="118"/>
-      <c r="U18" s="117"/>
-      <c r="V18" s="117"/>
-    </row>
-    <row r="19" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="90"/>
-      <c r="B19" s="106"/>
-      <c r="C19" s="107"/>
-      <c r="D19" s="107"/>
-      <c r="E19" s="119"/>
-      <c r="F19" s="108"/>
-      <c r="G19" s="109"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="97"/>
-      <c r="J19" s="111"/>
-      <c r="K19" s="112"/>
-      <c r="L19" s="113"/>
-      <c r="M19" s="114"/>
-      <c r="N19" s="112"/>
-      <c r="O19" s="112"/>
-      <c r="P19" s="113"/>
-      <c r="Q19" s="115"/>
-      <c r="R19" s="116"/>
-      <c r="S19" s="117"/>
-      <c r="T19" s="118"/>
-      <c r="U19" s="117"/>
-      <c r="V19" s="117"/>
-    </row>
-    <row r="20" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="90"/>
-      <c r="B20" s="106"/>
-      <c r="C20" s="107"/>
-      <c r="D20" s="107"/>
-      <c r="E20" s="119"/>
-      <c r="F20" s="108"/>
-      <c r="G20" s="109"/>
-      <c r="H20" s="110"/>
-      <c r="I20" s="97"/>
-      <c r="J20" s="111"/>
-      <c r="K20" s="112"/>
-      <c r="L20" s="113"/>
-      <c r="M20" s="114"/>
-      <c r="N20" s="112"/>
-      <c r="O20" s="112"/>
-      <c r="P20" s="113"/>
-      <c r="Q20" s="115"/>
-      <c r="R20" s="116"/>
-      <c r="S20" s="117"/>
-      <c r="T20" s="118"/>
-      <c r="U20" s="117"/>
-      <c r="V20" s="117"/>
-    </row>
-    <row r="21" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="90"/>
-      <c r="B21" s="106"/>
-      <c r="C21" s="107"/>
-      <c r="D21" s="92"/>
-      <c r="E21" s="93"/>
-      <c r="F21" s="108"/>
-      <c r="G21" s="109"/>
-      <c r="H21" s="110"/>
-      <c r="I21" s="97"/>
-      <c r="J21" s="111"/>
-      <c r="K21" s="112"/>
-      <c r="L21" s="113"/>
-      <c r="M21" s="114"/>
-      <c r="N21" s="112"/>
-      <c r="O21" s="112"/>
-      <c r="P21" s="113"/>
-      <c r="Q21" s="115"/>
-      <c r="R21" s="116"/>
-      <c r="S21" s="117"/>
-      <c r="T21" s="118"/>
-      <c r="U21" s="117"/>
-      <c r="V21" s="117"/>
-    </row>
-    <row r="22" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="90"/>
-      <c r="B22" s="106"/>
-      <c r="C22" s="107"/>
-      <c r="D22" s="92"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="108"/>
-      <c r="G22" s="109"/>
-      <c r="H22" s="110"/>
-      <c r="I22" s="97"/>
-      <c r="J22" s="111"/>
-      <c r="K22" s="112"/>
-      <c r="L22" s="113"/>
-      <c r="M22" s="114"/>
-      <c r="N22" s="112"/>
-      <c r="O22" s="112"/>
-      <c r="P22" s="113"/>
-      <c r="Q22" s="115"/>
-      <c r="R22" s="116"/>
-      <c r="S22" s="117"/>
-      <c r="T22" s="118"/>
-      <c r="U22" s="117"/>
-      <c r="V22" s="117"/>
-    </row>
-    <row r="23" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="90"/>
-      <c r="B23" s="106"/>
-      <c r="C23" s="107"/>
-      <c r="D23" s="107"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="108"/>
-      <c r="G23" s="109"/>
-      <c r="H23" s="110"/>
-      <c r="I23" s="97"/>
-      <c r="J23" s="111"/>
-      <c r="K23" s="112"/>
-      <c r="L23" s="113"/>
-      <c r="M23" s="114"/>
-      <c r="N23" s="112"/>
-      <c r="O23" s="112"/>
-      <c r="P23" s="113"/>
-      <c r="Q23" s="115"/>
-      <c r="R23" s="116"/>
-      <c r="S23" s="117"/>
-      <c r="T23" s="118"/>
-      <c r="U23" s="117"/>
-      <c r="V23" s="117"/>
-    </row>
-    <row r="24" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="90"/>
-      <c r="B24" s="106"/>
-      <c r="C24" s="107"/>
-      <c r="D24" s="107"/>
-      <c r="E24" s="93"/>
-      <c r="F24" s="108"/>
-      <c r="G24" s="109"/>
-      <c r="H24" s="110"/>
-      <c r="I24" s="97"/>
-      <c r="J24" s="111"/>
-      <c r="K24" s="112"/>
-      <c r="L24" s="113"/>
-      <c r="M24" s="114"/>
-      <c r="N24" s="112"/>
-      <c r="O24" s="112"/>
-      <c r="P24" s="113"/>
-      <c r="Q24" s="115"/>
-      <c r="R24" s="116"/>
-      <c r="S24" s="117"/>
-      <c r="T24" s="118"/>
-      <c r="U24" s="117"/>
-      <c r="V24" s="117"/>
-    </row>
-    <row r="25" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="90"/>
-      <c r="B25" s="106"/>
-      <c r="C25" s="107"/>
-      <c r="D25" s="107"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="108"/>
-      <c r="G25" s="109"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="97"/>
-      <c r="J25" s="111"/>
-      <c r="K25" s="112"/>
-      <c r="L25" s="113"/>
-      <c r="M25" s="114"/>
-      <c r="N25" s="112"/>
-      <c r="O25" s="112"/>
-      <c r="P25" s="113"/>
-      <c r="Q25" s="115"/>
-      <c r="R25" s="116"/>
-      <c r="S25" s="117"/>
-      <c r="T25" s="117"/>
-      <c r="U25" s="117"/>
-      <c r="V25" s="117"/>
-    </row>
-    <row r="26" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="90"/>
-      <c r="B26" s="106"/>
-      <c r="C26" s="107"/>
-      <c r="D26" s="107"/>
-      <c r="E26" s="119"/>
-      <c r="F26" s="108"/>
-      <c r="G26" s="109"/>
-      <c r="H26" s="110"/>
-      <c r="I26" s="97"/>
-      <c r="J26" s="111"/>
-      <c r="K26" s="112"/>
-      <c r="L26" s="113"/>
-      <c r="M26" s="114"/>
-      <c r="N26" s="112"/>
-      <c r="O26" s="112"/>
-      <c r="P26" s="113"/>
-      <c r="Q26" s="115"/>
-      <c r="R26" s="116"/>
-      <c r="S26" s="117"/>
-      <c r="T26" s="118"/>
-      <c r="U26" s="117"/>
-      <c r="V26" s="117"/>
-    </row>
-    <row r="27" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="90"/>
-      <c r="B27" s="106"/>
-      <c r="C27" s="107"/>
-      <c r="D27" s="107"/>
-      <c r="E27" s="119"/>
-      <c r="F27" s="108"/>
-      <c r="G27" s="109"/>
-      <c r="H27" s="110"/>
-      <c r="I27" s="97"/>
-      <c r="J27" s="111"/>
-      <c r="K27" s="112"/>
-      <c r="L27" s="113"/>
-      <c r="M27" s="114"/>
-      <c r="N27" s="112"/>
-      <c r="O27" s="112"/>
-      <c r="P27" s="113"/>
-      <c r="Q27" s="115"/>
-      <c r="R27" s="116"/>
-      <c r="S27" s="117"/>
-      <c r="T27" s="118"/>
-      <c r="U27" s="117"/>
-      <c r="V27" s="117"/>
-    </row>
-    <row r="28" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="90"/>
-      <c r="B28" s="106"/>
-      <c r="C28" s="107"/>
-      <c r="D28" s="107"/>
-      <c r="E28" s="119"/>
-      <c r="F28" s="108"/>
-      <c r="G28" s="109"/>
-      <c r="H28" s="110"/>
-      <c r="I28" s="97"/>
-      <c r="J28" s="111"/>
-      <c r="K28" s="112"/>
-      <c r="L28" s="113"/>
-      <c r="M28" s="114"/>
-      <c r="N28" s="112"/>
-      <c r="O28" s="112"/>
-      <c r="P28" s="113"/>
-      <c r="Q28" s="115"/>
-      <c r="R28" s="116"/>
-      <c r="S28" s="117"/>
-      <c r="T28" s="118"/>
-      <c r="U28" s="117"/>
-      <c r="V28" s="117"/>
-    </row>
-    <row r="29" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="90"/>
-      <c r="B29" s="106"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
-      <c r="E29" s="119"/>
-      <c r="F29" s="108"/>
-      <c r="G29" s="109"/>
-      <c r="H29" s="110"/>
-      <c r="I29" s="97"/>
-      <c r="J29" s="111"/>
-      <c r="K29" s="112"/>
-      <c r="L29" s="113"/>
-      <c r="M29" s="114"/>
-      <c r="N29" s="112"/>
-      <c r="O29" s="112"/>
-      <c r="P29" s="113"/>
-      <c r="Q29" s="115"/>
-      <c r="R29" s="116"/>
-      <c r="S29" s="117"/>
-      <c r="T29" s="118"/>
-      <c r="U29" s="117"/>
-      <c r="V29" s="117"/>
-    </row>
-    <row r="30" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="90"/>
-      <c r="B30" s="106"/>
-      <c r="C30" s="107"/>
-      <c r="D30" s="107"/>
-      <c r="E30" s="119"/>
-      <c r="F30" s="108"/>
-      <c r="G30" s="109"/>
-      <c r="H30" s="110"/>
-      <c r="I30" s="97"/>
-      <c r="J30" s="111"/>
-      <c r="K30" s="112"/>
-      <c r="L30" s="113"/>
-      <c r="M30" s="114"/>
-      <c r="N30" s="112"/>
-      <c r="O30" s="112"/>
-      <c r="P30" s="113"/>
-      <c r="Q30" s="115"/>
-      <c r="R30" s="116"/>
-      <c r="S30" s="117"/>
-      <c r="T30" s="118"/>
-      <c r="U30" s="117"/>
-      <c r="V30" s="117"/>
-    </row>
-    <row r="31" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="90"/>
-      <c r="B31" s="106"/>
-      <c r="C31" s="107"/>
-      <c r="D31" s="107"/>
-      <c r="E31" s="119"/>
-      <c r="F31" s="108"/>
-      <c r="G31" s="109"/>
-      <c r="H31" s="110"/>
-      <c r="I31" s="97"/>
-      <c r="J31" s="111"/>
-      <c r="K31" s="112"/>
-      <c r="L31" s="113"/>
-      <c r="M31" s="114"/>
-      <c r="N31" s="112"/>
-      <c r="O31" s="112"/>
-      <c r="P31" s="113"/>
-      <c r="Q31" s="115"/>
-      <c r="R31" s="116"/>
-      <c r="S31" s="117"/>
-      <c r="T31" s="118"/>
-      <c r="U31" s="117"/>
-      <c r="V31" s="117"/>
-    </row>
-    <row r="32" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="90"/>
-      <c r="B32" s="106"/>
-      <c r="C32" s="107"/>
-      <c r="D32" s="107"/>
-      <c r="E32" s="119"/>
-      <c r="F32" s="108"/>
-      <c r="G32" s="109"/>
-      <c r="H32" s="110"/>
-      <c r="I32" s="97"/>
-      <c r="J32" s="111"/>
-      <c r="K32" s="112"/>
-      <c r="L32" s="113"/>
-      <c r="M32" s="114"/>
-      <c r="N32" s="112"/>
-      <c r="O32" s="112"/>
-      <c r="P32" s="113"/>
-      <c r="Q32" s="115"/>
-      <c r="R32" s="116"/>
-      <c r="S32" s="117"/>
-      <c r="T32" s="118"/>
-      <c r="U32" s="117"/>
-      <c r="V32" s="117"/>
-    </row>
-    <row r="33" spans="1:39" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="90"/>
-      <c r="B33" s="106"/>
-      <c r="C33" s="107"/>
-      <c r="D33" s="107"/>
-      <c r="E33" s="119"/>
-      <c r="F33" s="108"/>
-      <c r="G33" s="109"/>
-      <c r="H33" s="110"/>
-      <c r="I33" s="97"/>
-      <c r="J33" s="111"/>
-      <c r="K33" s="112"/>
-      <c r="L33" s="113"/>
-      <c r="M33" s="114"/>
-      <c r="N33" s="112"/>
-      <c r="O33" s="112"/>
-      <c r="P33" s="113"/>
-      <c r="Q33" s="115"/>
-      <c r="R33" s="116"/>
-      <c r="S33" s="117"/>
-      <c r="T33" s="118"/>
-      <c r="U33" s="117"/>
-      <c r="V33" s="117"/>
-    </row>
-    <row r="34" spans="1:39" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="90"/>
-      <c r="B34" s="106"/>
-      <c r="C34" s="107"/>
-      <c r="D34" s="107"/>
-      <c r="E34" s="119"/>
-      <c r="F34" s="108"/>
-      <c r="G34" s="109"/>
-      <c r="H34" s="110"/>
-      <c r="I34" s="97"/>
-      <c r="J34" s="111"/>
-      <c r="K34" s="112"/>
-      <c r="L34" s="113"/>
-      <c r="M34" s="114"/>
-      <c r="N34" s="112"/>
-      <c r="O34" s="112"/>
-      <c r="P34" s="113"/>
-      <c r="Q34" s="115"/>
-      <c r="R34" s="116"/>
-      <c r="S34" s="117"/>
-      <c r="T34" s="118"/>
-      <c r="U34" s="117"/>
-      <c r="V34" s="117"/>
-    </row>
-    <row r="35" spans="1:39" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="90"/>
-      <c r="B35" s="106"/>
-      <c r="C35" s="107"/>
-      <c r="D35" s="107"/>
-      <c r="E35" s="119"/>
-      <c r="F35" s="108"/>
-      <c r="G35" s="109"/>
-      <c r="H35" s="110"/>
-      <c r="I35" s="97"/>
-      <c r="J35" s="111"/>
-      <c r="K35" s="112"/>
-      <c r="L35" s="113"/>
-      <c r="M35" s="114"/>
-      <c r="N35" s="112"/>
-      <c r="O35" s="112"/>
-      <c r="P35" s="113"/>
-      <c r="Q35" s="115"/>
-      <c r="R35" s="116"/>
-      <c r="S35" s="117"/>
-      <c r="T35" s="118"/>
-      <c r="U35" s="117"/>
-      <c r="V35" s="117"/>
-    </row>
-    <row r="36" spans="1:39" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="90"/>
-      <c r="B36" s="120"/>
-      <c r="C36" s="121"/>
-      <c r="D36" s="121"/>
-      <c r="E36" s="119"/>
-      <c r="F36" s="108"/>
-      <c r="G36" s="109"/>
-      <c r="H36" s="110"/>
-      <c r="I36" s="97"/>
-      <c r="J36" s="111"/>
-      <c r="K36" s="112"/>
-      <c r="L36" s="113"/>
-      <c r="M36" s="114"/>
-      <c r="N36" s="112"/>
-      <c r="O36" s="112"/>
-      <c r="P36" s="113"/>
-      <c r="Q36" s="115"/>
-      <c r="R36" s="116"/>
-      <c r="S36" s="117"/>
-      <c r="T36" s="118"/>
-      <c r="U36" s="117"/>
-      <c r="V36" s="117"/>
+      <c r="AI5" s="108"/>
+      <c r="AJ5" s="108"/>
+      <c r="AK5" s="108"/>
+      <c r="AL5" s="108"/>
+      <c r="AM5" s="108"/>
+      <c r="AN5" s="108"/>
+      <c r="AO5" s="108"/>
+      <c r="AP5" s="108"/>
+      <c r="AQ5" s="108"/>
+      <c r="AR5" s="108"/>
+      <c r="AS5" s="108"/>
+      <c r="AT5" s="108"/>
+      <c r="AU5" s="108"/>
+      <c r="AV5" s="108"/>
+    </row>
+    <row r="6" spans="1:48" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="53"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="66"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="68"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="AI6" s="108"/>
+      <c r="AJ6" s="108"/>
+      <c r="AK6" s="108"/>
+      <c r="AL6" s="108"/>
+      <c r="AM6" s="108"/>
+      <c r="AN6" s="108"/>
+      <c r="AO6" s="108"/>
+      <c r="AP6" s="108"/>
+      <c r="AQ6" s="108"/>
+      <c r="AR6" s="108"/>
+      <c r="AS6" s="108"/>
+      <c r="AT6" s="108"/>
+      <c r="AU6" s="108"/>
+      <c r="AV6" s="108"/>
+    </row>
+    <row r="7" spans="1:48" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="53"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="AI7" s="108"/>
+      <c r="AJ7" s="108"/>
+      <c r="AK7" s="108"/>
+      <c r="AL7" s="108"/>
+      <c r="AM7" s="108"/>
+      <c r="AN7" s="108"/>
+      <c r="AO7" s="108"/>
+      <c r="AP7" s="108"/>
+      <c r="AQ7" s="108"/>
+      <c r="AR7" s="108"/>
+      <c r="AS7" s="108"/>
+      <c r="AT7" s="108"/>
+      <c r="AU7" s="108"/>
+      <c r="AV7" s="108"/>
+    </row>
+    <row r="8" spans="1:48" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="53"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="AI8" s="108"/>
+      <c r="AJ8" s="108"/>
+      <c r="AK8" s="108"/>
+      <c r="AL8" s="108"/>
+      <c r="AM8" s="108"/>
+      <c r="AN8" s="108"/>
+      <c r="AO8" s="108"/>
+      <c r="AP8" s="108"/>
+      <c r="AQ8" s="108"/>
+      <c r="AR8" s="108"/>
+      <c r="AS8" s="108"/>
+      <c r="AT8" s="108"/>
+      <c r="AU8" s="108"/>
+      <c r="AV8" s="108"/>
+    </row>
+    <row r="9" spans="1:48" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="53"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="AI9" s="108"/>
+      <c r="AJ9" s="108"/>
+      <c r="AK9" s="108"/>
+      <c r="AL9" s="108"/>
+      <c r="AM9" s="108"/>
+      <c r="AN9" s="108"/>
+      <c r="AO9" s="108"/>
+      <c r="AP9" s="108"/>
+      <c r="AQ9" s="108"/>
+      <c r="AR9" s="108"/>
+      <c r="AS9" s="108"/>
+      <c r="AT9" s="108"/>
+      <c r="AU9" s="108"/>
+      <c r="AV9" s="108"/>
+    </row>
+    <row r="10" spans="1:48" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="53"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="AI10" s="108"/>
+      <c r="AJ10" s="108"/>
+      <c r="AK10" s="108"/>
+      <c r="AL10" s="108"/>
+      <c r="AM10" s="108"/>
+      <c r="AN10" s="108"/>
+      <c r="AO10" s="108"/>
+      <c r="AP10" s="108"/>
+      <c r="AQ10" s="108"/>
+      <c r="AR10" s="108"/>
+      <c r="AS10" s="108"/>
+      <c r="AT10" s="108"/>
+      <c r="AU10" s="108"/>
+      <c r="AV10" s="108"/>
+    </row>
+    <row r="11" spans="1:48" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="53"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="28"/>
+      <c r="V11" s="28"/>
+      <c r="AI11" s="108"/>
+      <c r="AJ11" s="108"/>
+      <c r="AK11" s="108"/>
+      <c r="AL11" s="108"/>
+      <c r="AM11" s="108"/>
+      <c r="AN11" s="108"/>
+      <c r="AO11" s="108"/>
+      <c r="AP11" s="108"/>
+      <c r="AQ11" s="108"/>
+      <c r="AR11" s="108"/>
+      <c r="AS11" s="108"/>
+      <c r="AT11" s="108"/>
+      <c r="AU11" s="108"/>
+      <c r="AV11" s="108"/>
+    </row>
+    <row r="12" spans="1:48" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A12" s="53"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="AJ12" s="74"/>
+      <c r="AK12" s="74"/>
+      <c r="AL12" s="74"/>
+      <c r="AM12" s="74"/>
+      <c r="AN12" s="74"/>
+      <c r="AO12" s="74"/>
+      <c r="AP12" s="74"/>
+      <c r="AQ12" s="74"/>
+      <c r="AR12" s="74"/>
+      <c r="AS12" s="74"/>
+      <c r="AT12" s="74"/>
+      <c r="AU12" s="74"/>
+      <c r="AV12" s="74"/>
+    </row>
+    <row r="13" spans="1:48" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A13" s="53"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="AJ13" s="75"/>
+      <c r="AK13" s="75"/>
+      <c r="AL13" s="75"/>
+      <c r="AM13" s="75"/>
+      <c r="AN13" s="75"/>
+      <c r="AO13" s="75"/>
+      <c r="AP13" s="75"/>
+      <c r="AQ13" s="75"/>
+      <c r="AR13" s="75"/>
+      <c r="AS13" s="75"/>
+      <c r="AT13" s="75"/>
+      <c r="AU13" s="75"/>
+      <c r="AV13" s="75"/>
+    </row>
+    <row r="14" spans="1:48" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A14" s="53"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="AJ14" s="75"/>
+      <c r="AK14" s="75"/>
+      <c r="AL14" s="75"/>
+      <c r="AM14" s="75"/>
+      <c r="AN14" s="75"/>
+      <c r="AO14" s="75"/>
+      <c r="AP14" s="75"/>
+      <c r="AQ14" s="75"/>
+      <c r="AR14" s="75"/>
+      <c r="AS14" s="75"/>
+      <c r="AT14" s="75"/>
+      <c r="AU14" s="75"/>
+      <c r="AV14" s="75"/>
+    </row>
+    <row r="15" spans="1:48" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="53"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+    </row>
+    <row r="16" spans="1:48" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="53"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+    </row>
+    <row r="17" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="53"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="28"/>
+      <c r="V17" s="28"/>
+    </row>
+    <row r="18" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="53"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="25"/>
+      <c r="U18" s="28"/>
+      <c r="V18" s="28"/>
+    </row>
+    <row r="19" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="53"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="25"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+    </row>
+    <row r="20" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="53"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="25"/>
+      <c r="U20" s="28"/>
+      <c r="V20" s="28"/>
+    </row>
+    <row r="21" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="53"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="25"/>
+      <c r="U21" s="28"/>
+      <c r="V21" s="28"/>
+    </row>
+    <row r="22" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="53"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="34"/>
+      <c r="S22" s="28"/>
+      <c r="T22" s="25"/>
+      <c r="U22" s="28"/>
+      <c r="V22" s="28"/>
+    </row>
+    <row r="23" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="53"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="28"/>
+      <c r="T23" s="25"/>
+      <c r="U23" s="28"/>
+      <c r="V23" s="28"/>
+    </row>
+    <row r="24" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="53"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="28"/>
+    </row>
+    <row r="25" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="53"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="34"/>
+      <c r="S25" s="28"/>
+      <c r="T25" s="28"/>
+      <c r="U25" s="28"/>
+      <c r="V25" s="28"/>
+    </row>
+    <row r="26" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="53"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="34"/>
+      <c r="S26" s="28"/>
+      <c r="T26" s="25"/>
+      <c r="U26" s="28"/>
+      <c r="V26" s="28"/>
+    </row>
+    <row r="27" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="53"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="73"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="34"/>
+      <c r="S27" s="28"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="28"/>
+      <c r="V27" s="28"/>
+    </row>
+    <row r="28" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="53"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="73"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="34"/>
+      <c r="S28" s="28"/>
+      <c r="T28" s="25"/>
+      <c r="U28" s="28"/>
+      <c r="V28" s="28"/>
+    </row>
+    <row r="29" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="53"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="73"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="34"/>
+      <c r="S29" s="28"/>
+      <c r="T29" s="25"/>
+      <c r="U29" s="28"/>
+      <c r="V29" s="28"/>
+    </row>
+    <row r="30" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="53"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="73"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="34"/>
+      <c r="S30" s="28"/>
+      <c r="T30" s="25"/>
+      <c r="U30" s="28"/>
+      <c r="V30" s="28"/>
+    </row>
+    <row r="31" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="53"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="73"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="34"/>
+      <c r="S31" s="28"/>
+      <c r="T31" s="25"/>
+      <c r="U31" s="28"/>
+      <c r="V31" s="28"/>
+    </row>
+    <row r="32" spans="1:22" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="53"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="73"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="34"/>
+      <c r="S32" s="28"/>
+      <c r="T32" s="25"/>
+      <c r="U32" s="28"/>
+      <c r="V32" s="28"/>
+    </row>
+    <row r="33" spans="1:39" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="53"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="34"/>
+      <c r="S33" s="28"/>
+      <c r="T33" s="25"/>
+      <c r="U33" s="28"/>
+      <c r="V33" s="28"/>
+    </row>
+    <row r="34" spans="1:39" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="53"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="34"/>
+      <c r="S34" s="28"/>
+      <c r="T34" s="25"/>
+      <c r="U34" s="28"/>
+      <c r="V34" s="28"/>
+    </row>
+    <row r="35" spans="1:39" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="53"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="72"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="73"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="34"/>
+      <c r="S35" s="28"/>
+      <c r="T35" s="25"/>
+      <c r="U35" s="28"/>
+      <c r="V35" s="28"/>
+    </row>
+    <row r="36" spans="1:39" s="6" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="53"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="60"/>
+      <c r="J36" s="73"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="34"/>
+      <c r="S36" s="28"/>
+      <c r="T36" s="25"/>
+      <c r="U36" s="28"/>
+      <c r="V36" s="28"/>
     </row>
     <row r="37" spans="1:39" ht="28.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="67" t="s">
+      <c r="A37" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="68"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="62">
+      <c r="B37" s="100"/>
+      <c r="C37" s="100"/>
+      <c r="D37" s="94">
         <f>H37+J37+K37+L37+M37+N37+O37+P37+S37+T37+U37+V37</f>
         <v>0</v>
       </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="17">
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="22">
         <f>SUM(H6:H36)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="18"/>
-      <c r="J37" s="19">
+      <c r="I37" s="23"/>
+      <c r="J37" s="24">
         <f t="shared" ref="J37:V37" si="0">SUM(J6:J36)</f>
         <v>0</v>
       </c>
-      <c r="K37" s="19">
+      <c r="K37" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L37" s="19">
+      <c r="L37" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M37" s="19">
+      <c r="M37" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N37" s="19">
+      <c r="N37" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O37" s="19">
+      <c r="O37" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P37" s="19">
+      <c r="P37" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q37" s="47">
+      <c r="Q37" s="79">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R37" s="47">
+      <c r="R37" s="79">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S37" s="20">
+      <c r="S37" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T37" s="20">
+      <c r="T37" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U37" s="20">
+      <c r="U37" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V37" s="20">
+      <c r="V37" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W37" s="5"/>
-      <c r="X37" s="5"/>
-      <c r="Y37" s="5"/>
-      <c r="Z37" s="5"/>
-      <c r="AA37" s="5"/>
-      <c r="AB37" s="5"/>
-      <c r="AC37" s="5"/>
-      <c r="AD37" s="5"/>
-      <c r="AE37" s="5"/>
-      <c r="AF37" s="5"/>
-      <c r="AG37" s="5"/>
-      <c r="AH37" s="5"/>
-      <c r="AI37" s="5"/>
-      <c r="AJ37" s="5"/>
-      <c r="AK37" s="5"/>
-      <c r="AL37" s="5"/>
-      <c r="AM37" s="5"/>
+      <c r="W37" s="7"/>
+      <c r="X37" s="7"/>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="7"/>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7"/>
+      <c r="AC37" s="7"/>
+      <c r="AD37" s="7"/>
+      <c r="AE37" s="7"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="7"/>
+      <c r="AJ37" s="7"/>
+      <c r="AK37" s="7"/>
+      <c r="AL37" s="7"/>
+      <c r="AM37" s="7"/>
     </row>
     <row r="38" spans="1:39" ht="19.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="63"/>
-      <c r="H38" s="13" t="s">
+      <c r="B38" s="82"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="95"/>
+      <c r="H38" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I38" s="46"/>
-      <c r="J38" s="15" t="s">
+      <c r="I38" s="78"/>
+      <c r="J38" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="K38" s="15" t="s">
+      <c r="K38" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="L38" s="15" t="s">
+      <c r="L38" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="M38" s="15" t="s">
+      <c r="M38" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="N38" s="15" t="s">
+      <c r="N38" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="O38" s="15" t="s">
+      <c r="O38" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="P38" s="15" t="s">
+      <c r="P38" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q38" s="48"/>
-      <c r="R38" s="48"/>
-      <c r="S38" s="22" t="s">
+      <c r="Q38" s="80"/>
+      <c r="R38" s="80"/>
+      <c r="S38" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="T38" s="22" t="s">
+      <c r="T38" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="U38" s="22" t="s">
+      <c r="U38" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="V38" s="22" t="s">
+      <c r="V38" s="29" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Colorazione grigia weekend + festivita
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesho\Desktop\ore\ore-pws\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B32D81-9211-4DB9-B468-BF50B9B025C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF139C55-9FE7-4BD5-AA6E-6EF7C5738A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>ORE ORDINARIE</t>
   </si>
@@ -144,12 +144,6 @@
   </si>
   <si>
     <t>(N)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEONID LYAKHU  </t>
-  </si>
-  <si>
-    <t>GENNAIO 2026</t>
   </si>
 </sst>
 </file>
@@ -160,7 +154,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +313,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -970,7 +970,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -992,12 +992,6 @@
     <xf numFmtId="4" fontId="13" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="13" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="13" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1009,11 +1003,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="17" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="12" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="19" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="20" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="18" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="18" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1083,14 +1073,96 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="12" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="18" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="19" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="17" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="20" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1118,7 +1190,9 @@
     <xf numFmtId="2" fontId="21" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="4" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1129,7 +1203,9 @@
     <xf numFmtId="2" fontId="9" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1144,12 +1220,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="19" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1177,19 +1247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1509,61 +1567,63 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AV37"/>
+  <dimension ref="A1:AX37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="8" ySplit="4" topLeftCell="I5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="4" topLeftCell="AI5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="AL11" sqref="AL11:AW14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" style="24" customWidth="1"/>
     <col min="3" max="3" width="22" style="7" customWidth="1"/>
     <col min="4" max="4" width="22.109375" style="7" customWidth="1"/>
-    <col min="5" max="7" width="8.77734375" style="15" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" style="19" customWidth="1"/>
-    <col min="9" max="9" width="8.77734375" style="17" customWidth="1"/>
-    <col min="10" max="15" width="8.77734375" style="19" customWidth="1"/>
-    <col min="16" max="16" width="10.5546875" style="19" customWidth="1"/>
+    <col min="5" max="7" width="8.77734375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" style="17" customWidth="1"/>
+    <col min="9" max="9" width="3.33203125" style="15" customWidth="1"/>
+    <col min="10" max="15" width="8.77734375" style="17" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" style="17" customWidth="1"/>
     <col min="17" max="17" width="5.44140625" customWidth="1"/>
-    <col min="18" max="18" width="6" style="32" customWidth="1"/>
-    <col min="19" max="19" width="7" style="28" customWidth="1"/>
-    <col min="20" max="20" width="8.109375" style="25" customWidth="1"/>
-    <col min="21" max="21" width="10.88671875" style="28" customWidth="1"/>
-    <col min="22" max="22" width="10.21875" style="28" customWidth="1"/>
+    <col min="18" max="18" width="6" style="26" customWidth="1"/>
+    <col min="19" max="19" width="7" style="22" customWidth="1"/>
+    <col min="20" max="20" width="8.109375" style="19" customWidth="1"/>
+    <col min="21" max="21" width="10.88671875" style="22" customWidth="1"/>
+    <col min="22" max="22" width="10.21875" style="22" customWidth="1"/>
+    <col min="23" max="23" width="0.44140625" customWidth="1"/>
+    <col min="24" max="24" width="0.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="60"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="90" t="s">
+    <row r="1" spans="1:50" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="80"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="62"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="82"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="62"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81"/>
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="82"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
@@ -1576,74 +1636,72 @@
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
-      <c r="AI1" s="85" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ1" s="86"/>
-      <c r="AK1" s="86"/>
-      <c r="AL1" s="86"/>
-      <c r="AM1" s="86"/>
-      <c r="AN1" s="86"/>
-      <c r="AO1" s="86"/>
-      <c r="AP1" s="86"/>
-      <c r="AQ1" s="86"/>
-      <c r="AR1" s="86"/>
-      <c r="AS1" s="86"/>
-      <c r="AT1" s="86"/>
-      <c r="AU1" s="86"/>
-      <c r="AV1" s="86"/>
-    </row>
-    <row r="2" spans="1:48" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="79" t="s">
+      <c r="AK1" s="118"/>
+      <c r="AL1" s="118"/>
+      <c r="AM1" s="118"/>
+      <c r="AN1" s="118"/>
+      <c r="AO1" s="118"/>
+      <c r="AP1" s="118"/>
+      <c r="AQ1" s="118"/>
+      <c r="AR1" s="118"/>
+      <c r="AS1" s="118"/>
+      <c r="AT1" s="118"/>
+      <c r="AU1" s="118"/>
+      <c r="AV1" s="118"/>
+      <c r="AW1" s="118"/>
+      <c r="AX1" s="118"/>
+    </row>
+    <row r="2" spans="1:50" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="70" t="s">
+      <c r="E2" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="94" t="s">
+      <c r="F2" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="70" t="s">
+      <c r="G2" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="95" t="s">
+      <c r="H2" s="113" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="9"/>
-      <c r="J2" s="67" t="s">
+      <c r="J2" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="61"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="76" t="s">
+      <c r="K2" s="81"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="96" t="s">
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="97"/>
-      <c r="S2" s="87" t="s">
+      <c r="R2" s="115"/>
+      <c r="S2" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="83" t="s">
+      <c r="T2" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="63" t="s">
+      <c r="U2" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="83" t="s">
+      <c r="V2" s="103" t="s">
         <v>15</v>
       </c>
       <c r="W2" s="2"/>
@@ -1658,58 +1716,58 @@
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
-      <c r="AI2" s="86"/>
-      <c r="AJ2" s="86"/>
-      <c r="AK2" s="86"/>
-      <c r="AL2" s="86"/>
-      <c r="AM2" s="86"/>
-      <c r="AN2" s="86"/>
-      <c r="AO2" s="86"/>
-      <c r="AP2" s="86"/>
-      <c r="AQ2" s="86"/>
-      <c r="AR2" s="86"/>
-      <c r="AS2" s="86"/>
-      <c r="AT2" s="86"/>
-      <c r="AU2" s="86"/>
-      <c r="AV2" s="86"/>
-    </row>
-    <row r="3" spans="1:48" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="80"/>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
+      <c r="AK2" s="118"/>
+      <c r="AL2" s="118"/>
+      <c r="AM2" s="118"/>
+      <c r="AN2" s="118"/>
+      <c r="AO2" s="118"/>
+      <c r="AP2" s="118"/>
+      <c r="AQ2" s="118"/>
+      <c r="AR2" s="118"/>
+      <c r="AS2" s="118"/>
+      <c r="AT2" s="118"/>
+      <c r="AU2" s="118"/>
+      <c r="AV2" s="118"/>
+      <c r="AW2" s="118"/>
+      <c r="AX2" s="118"/>
+    </row>
+    <row r="3" spans="1:50" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="100"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="74" t="s">
+      <c r="J3" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="92" t="s">
+      <c r="K3" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="81" t="s">
+      <c r="L3" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="74" t="s">
+      <c r="M3" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="92" t="s">
+      <c r="N3" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="81" t="s">
+      <c r="O3" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="68" t="s">
+      <c r="P3" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="98"/>
-      <c r="R3" s="99"/>
-      <c r="S3" s="88"/>
-      <c r="T3" s="71"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="71"/>
+      <c r="Q3" s="116"/>
+      <c r="R3" s="117"/>
+      <c r="S3" s="106"/>
+      <c r="T3" s="91"/>
+      <c r="U3" s="84"/>
+      <c r="V3" s="91"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
@@ -1722,48 +1780,48 @@
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
-      <c r="AI3" s="86"/>
-      <c r="AJ3" s="86"/>
-      <c r="AK3" s="86"/>
-      <c r="AL3" s="86"/>
-      <c r="AM3" s="86"/>
-      <c r="AN3" s="86"/>
-      <c r="AO3" s="86"/>
-      <c r="AP3" s="86"/>
-      <c r="AQ3" s="86"/>
-      <c r="AR3" s="86"/>
-      <c r="AS3" s="86"/>
-      <c r="AT3" s="86"/>
-      <c r="AU3" s="86"/>
-      <c r="AV3" s="86"/>
-    </row>
-    <row r="4" spans="1:48" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="75"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
+      <c r="AK3" s="118"/>
+      <c r="AL3" s="118"/>
+      <c r="AM3" s="118"/>
+      <c r="AN3" s="118"/>
+      <c r="AO3" s="118"/>
+      <c r="AP3" s="118"/>
+      <c r="AQ3" s="118"/>
+      <c r="AR3" s="118"/>
+      <c r="AS3" s="118"/>
+      <c r="AT3" s="118"/>
+      <c r="AU3" s="118"/>
+      <c r="AV3" s="118"/>
+      <c r="AW3" s="118"/>
+      <c r="AX3" s="118"/>
+    </row>
+    <row r="4" spans="1:50" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="95"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
       <c r="I4" s="9"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="69"/>
-      <c r="Q4" s="103" t="s">
+      <c r="J4" s="95"/>
+      <c r="K4" s="111"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="111"/>
+      <c r="O4" s="102"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="104" t="s">
+      <c r="R4" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="S4" s="89"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="65"/>
-      <c r="V4" s="69"/>
+      <c r="S4" s="107"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="85"/>
+      <c r="V4" s="89"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -1776,70 +1834,72 @@
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="86"/>
-      <c r="AK4" s="86"/>
-      <c r="AL4" s="86"/>
-      <c r="AM4" s="86"/>
-      <c r="AN4" s="86"/>
-      <c r="AO4" s="86"/>
-      <c r="AP4" s="86"/>
-      <c r="AQ4" s="86"/>
-      <c r="AR4" s="86"/>
-      <c r="AS4" s="86"/>
-      <c r="AT4" s="86"/>
-      <c r="AU4" s="86"/>
-      <c r="AV4" s="86"/>
-    </row>
-    <row r="5" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="47"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="AI5" s="86"/>
-      <c r="AJ5" s="86"/>
-      <c r="AK5" s="86"/>
-      <c r="AL5" s="86"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="86"/>
-      <c r="AO5" s="86"/>
-      <c r="AP5" s="86"/>
-      <c r="AQ5" s="86"/>
-      <c r="AR5" s="86"/>
-      <c r="AS5" s="86"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="86"/>
-      <c r="AV5" s="86"/>
-    </row>
-    <row r="6" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="33"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="52"/>
+      <c r="AK4" s="118"/>
+      <c r="AL4" s="118"/>
+      <c r="AM4" s="118"/>
+      <c r="AN4" s="118"/>
+      <c r="AO4" s="118"/>
+      <c r="AP4" s="118"/>
+      <c r="AQ4" s="118"/>
+      <c r="AR4" s="118"/>
+      <c r="AS4" s="118"/>
+      <c r="AT4" s="118"/>
+      <c r="AU4" s="118"/>
+      <c r="AV4" s="118"/>
+      <c r="AW4" s="118"/>
+      <c r="AX4" s="118"/>
+    </row>
+    <row r="5" spans="1:50" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="27"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="AI5"/>
+      <c r="AJ5"/>
+      <c r="AK5" s="118"/>
+      <c r="AL5" s="118"/>
+      <c r="AM5" s="118"/>
+      <c r="AN5" s="118"/>
+      <c r="AO5" s="118"/>
+      <c r="AP5" s="118"/>
+      <c r="AQ5" s="118"/>
+      <c r="AR5" s="118"/>
+      <c r="AS5" s="118"/>
+      <c r="AT5" s="118"/>
+      <c r="AU5" s="118"/>
+      <c r="AV5" s="118"/>
+      <c r="AW5" s="118"/>
+      <c r="AX5" s="118"/>
+    </row>
+    <row r="6" spans="1:50" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="27"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="46"/>
       <c r="K6" s="10"/>
       <c r="L6" s="11"/>
       <c r="M6" s="12"/>
@@ -1847,37 +1907,39 @@
       <c r="O6" s="10"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="3"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="26"/>
-      <c r="AI6" s="86"/>
-      <c r="AJ6" s="86"/>
-      <c r="AK6" s="86"/>
-      <c r="AL6" s="86"/>
-      <c r="AM6" s="86"/>
-      <c r="AN6" s="86"/>
-      <c r="AO6" s="86"/>
-      <c r="AP6" s="86"/>
-      <c r="AQ6" s="86"/>
-      <c r="AR6" s="86"/>
-      <c r="AS6" s="86"/>
-      <c r="AT6" s="86"/>
-      <c r="AU6" s="86"/>
-      <c r="AV6" s="86"/>
-    </row>
-    <row r="7" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="33"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="52"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+      <c r="AI6"/>
+      <c r="AJ6"/>
+      <c r="AK6" s="118"/>
+      <c r="AL6" s="118"/>
+      <c r="AM6" s="118"/>
+      <c r="AN6" s="118"/>
+      <c r="AO6" s="118"/>
+      <c r="AP6" s="118"/>
+      <c r="AQ6" s="118"/>
+      <c r="AR6" s="118"/>
+      <c r="AS6" s="118"/>
+      <c r="AT6" s="118"/>
+      <c r="AU6" s="118"/>
+      <c r="AV6" s="118"/>
+      <c r="AW6" s="118"/>
+      <c r="AX6" s="118"/>
+    </row>
+    <row r="7" spans="1:50" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="27"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="46"/>
       <c r="K7" s="10"/>
       <c r="L7" s="11"/>
       <c r="M7" s="12"/>
@@ -1885,37 +1947,39 @@
       <c r="O7" s="10"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="3"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="26"/>
-      <c r="AI7" s="86"/>
-      <c r="AJ7" s="86"/>
-      <c r="AK7" s="86"/>
-      <c r="AL7" s="86"/>
-      <c r="AM7" s="86"/>
-      <c r="AN7" s="86"/>
-      <c r="AO7" s="86"/>
-      <c r="AP7" s="86"/>
-      <c r="AQ7" s="86"/>
-      <c r="AR7" s="86"/>
-      <c r="AS7" s="86"/>
-      <c r="AT7" s="86"/>
-      <c r="AU7" s="86"/>
-      <c r="AV7" s="86"/>
-    </row>
-    <row r="8" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="33"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="52"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="AI7"/>
+      <c r="AJ7"/>
+      <c r="AK7" s="118"/>
+      <c r="AL7" s="118"/>
+      <c r="AM7" s="118"/>
+      <c r="AN7" s="118"/>
+      <c r="AO7" s="118"/>
+      <c r="AP7" s="118"/>
+      <c r="AQ7" s="118"/>
+      <c r="AR7" s="118"/>
+      <c r="AS7" s="118"/>
+      <c r="AT7" s="118"/>
+      <c r="AU7" s="118"/>
+      <c r="AV7" s="118"/>
+      <c r="AW7" s="118"/>
+      <c r="AX7" s="118"/>
+    </row>
+    <row r="8" spans="1:50" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="27"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="46"/>
       <c r="K8" s="10"/>
       <c r="L8" s="11"/>
       <c r="M8" s="12"/>
@@ -1923,37 +1987,39 @@
       <c r="O8" s="10"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="3"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="26"/>
-      <c r="V8" s="26"/>
-      <c r="AI8" s="86"/>
-      <c r="AJ8" s="86"/>
-      <c r="AK8" s="86"/>
-      <c r="AL8" s="86"/>
-      <c r="AM8" s="86"/>
-      <c r="AN8" s="86"/>
-      <c r="AO8" s="86"/>
-      <c r="AP8" s="86"/>
-      <c r="AQ8" s="86"/>
-      <c r="AR8" s="86"/>
-      <c r="AS8" s="86"/>
-      <c r="AT8" s="86"/>
-      <c r="AU8" s="86"/>
-      <c r="AV8" s="86"/>
-    </row>
-    <row r="9" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="33"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="52"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="AI8"/>
+      <c r="AJ8"/>
+      <c r="AK8" s="118"/>
+      <c r="AL8" s="118"/>
+      <c r="AM8" s="118"/>
+      <c r="AN8" s="118"/>
+      <c r="AO8" s="118"/>
+      <c r="AP8" s="118"/>
+      <c r="AQ8" s="118"/>
+      <c r="AR8" s="118"/>
+      <c r="AS8" s="118"/>
+      <c r="AT8" s="118"/>
+      <c r="AU8" s="118"/>
+      <c r="AV8" s="118"/>
+      <c r="AW8" s="118"/>
+      <c r="AX8" s="118"/>
+    </row>
+    <row r="9" spans="1:50" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="27"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="46"/>
       <c r="K9" s="10"/>
       <c r="L9" s="11"/>
       <c r="M9" s="12"/>
@@ -1961,780 +2027,789 @@
       <c r="O9" s="10"/>
       <c r="P9" s="11"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="26"/>
-      <c r="V9" s="26"/>
-      <c r="AI9" s="86"/>
-      <c r="AJ9" s="86"/>
-      <c r="AK9" s="86"/>
-      <c r="AL9" s="86"/>
-      <c r="AM9" s="86"/>
-      <c r="AN9" s="86"/>
-      <c r="AO9" s="86"/>
-      <c r="AP9" s="86"/>
-      <c r="AQ9" s="86"/>
-      <c r="AR9" s="86"/>
-      <c r="AS9" s="86"/>
-      <c r="AT9" s="86"/>
-      <c r="AU9" s="86"/>
-      <c r="AV9" s="86"/>
-    </row>
-    <row r="10" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="33"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="26"/>
-      <c r="V10" s="26"/>
-      <c r="AI10" s="86"/>
-      <c r="AJ10" s="86"/>
-      <c r="AK10" s="86"/>
-      <c r="AL10" s="86"/>
-      <c r="AM10" s="86"/>
-      <c r="AN10" s="86"/>
-      <c r="AO10" s="86"/>
-      <c r="AP10" s="86"/>
-      <c r="AQ10" s="86"/>
-      <c r="AR10" s="86"/>
-      <c r="AS10" s="86"/>
-      <c r="AT10" s="86"/>
-      <c r="AU10" s="86"/>
-      <c r="AV10" s="86"/>
-    </row>
-    <row r="11" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A11" s="33"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="26"/>
-      <c r="V11" s="26"/>
-      <c r="AJ11" s="53"/>
-      <c r="AK11" s="53"/>
-      <c r="AL11" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM11" s="57"/>
-      <c r="AN11" s="57"/>
-      <c r="AO11" s="57"/>
-      <c r="AP11" s="57"/>
-      <c r="AQ11" s="57"/>
-      <c r="AR11" s="57"/>
-      <c r="AS11" s="57"/>
-      <c r="AT11" s="53"/>
-      <c r="AU11" s="53"/>
-      <c r="AV11" s="53"/>
-    </row>
-    <row r="12" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A12" s="33"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="26"/>
-      <c r="V12" s="26"/>
-      <c r="AJ12" s="54"/>
-      <c r="AK12" s="54"/>
-      <c r="AL12" s="57"/>
-      <c r="AM12" s="57"/>
-      <c r="AN12" s="57"/>
-      <c r="AO12" s="57"/>
-      <c r="AP12" s="57"/>
-      <c r="AQ12" s="57"/>
-      <c r="AR12" s="57"/>
-      <c r="AS12" s="57"/>
-      <c r="AT12" s="54"/>
-      <c r="AU12" s="54"/>
-      <c r="AV12" s="54"/>
-    </row>
-    <row r="13" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A13" s="33"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="26"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="26"/>
-      <c r="V13" s="26"/>
-      <c r="AJ13" s="54"/>
-      <c r="AK13" s="54"/>
-      <c r="AL13" s="57"/>
-      <c r="AM13" s="57"/>
-      <c r="AN13" s="57"/>
-      <c r="AO13" s="57"/>
-      <c r="AP13" s="57"/>
-      <c r="AQ13" s="57"/>
-      <c r="AR13" s="57"/>
-      <c r="AS13" s="57"/>
-      <c r="AT13" s="54"/>
-      <c r="AU13" s="54"/>
-      <c r="AV13" s="54"/>
-    </row>
-    <row r="14" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="33"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="26"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="26"/>
-      <c r="V14" s="26"/>
-      <c r="AL14" s="57"/>
-      <c r="AM14" s="57"/>
-      <c r="AN14" s="57"/>
-      <c r="AO14" s="57"/>
-      <c r="AP14" s="57"/>
-      <c r="AQ14" s="57"/>
-      <c r="AR14" s="57"/>
-      <c r="AS14" s="57"/>
-    </row>
-    <row r="15" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="33"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="26"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="26"/>
-      <c r="V15" s="26"/>
-    </row>
-    <row r="16" spans="1:48" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="33"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="31"/>
-      <c r="S16" s="26"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="26"/>
-      <c r="V16" s="26"/>
-    </row>
-    <row r="17" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="33"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="31"/>
-      <c r="S17" s="26"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="26"/>
-      <c r="V17" s="26"/>
-    </row>
-    <row r="18" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="33"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="31"/>
-      <c r="S18" s="26"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="26"/>
-      <c r="V18" s="26"/>
-    </row>
-    <row r="19" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="33"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="31"/>
-      <c r="S19" s="26"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="26"/>
-      <c r="V19" s="26"/>
-    </row>
-    <row r="20" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="33"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="31"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="26"/>
-      <c r="V20" s="26"/>
-    </row>
-    <row r="21" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="33"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="31"/>
-      <c r="S21" s="26"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="26"/>
-    </row>
-    <row r="22" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="33"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="31"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="23"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="26"/>
-    </row>
-    <row r="23" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="33"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="31"/>
-      <c r="S23" s="26"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="26"/>
-      <c r="V23" s="26"/>
-    </row>
-    <row r="24" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="33"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="101"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="31"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
-    </row>
-    <row r="25" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="33"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="31"/>
-      <c r="S25" s="26"/>
-      <c r="T25" s="23"/>
-      <c r="U25" s="26"/>
-      <c r="V25" s="26"/>
-    </row>
-    <row r="26" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="33"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="101"/>
-      <c r="D26" s="101"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="31"/>
-      <c r="S26" s="26"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="26"/>
-      <c r="V26" s="26"/>
-    </row>
-    <row r="27" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="33"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="101"/>
-      <c r="D27" s="101"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="31"/>
-      <c r="S27" s="26"/>
-      <c r="T27" s="23"/>
-      <c r="U27" s="26"/>
-      <c r="V27" s="26"/>
-    </row>
-    <row r="28" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="33"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="101"/>
-      <c r="D28" s="101"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="31"/>
-      <c r="S28" s="26"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="26"/>
-      <c r="V28" s="26"/>
-    </row>
-    <row r="29" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="33"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="101"/>
-      <c r="D29" s="101"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="31"/>
-      <c r="S29" s="26"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="26"/>
-      <c r="V29" s="26"/>
-    </row>
-    <row r="30" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="33"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="101"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="31"/>
-      <c r="S30" s="26"/>
-      <c r="T30" s="23"/>
-      <c r="U30" s="26"/>
-      <c r="V30" s="26"/>
-    </row>
-    <row r="31" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="33"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="101"/>
-      <c r="D31" s="101"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="52"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="31"/>
-      <c r="S31" s="26"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="26"/>
-      <c r="V31" s="26"/>
-    </row>
-    <row r="32" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="33"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="101"/>
-      <c r="D32" s="101"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="51"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="31"/>
-      <c r="S32" s="26"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="26"/>
-      <c r="V32" s="26"/>
-    </row>
-    <row r="33" spans="1:39" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="33"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="101"/>
-      <c r="D33" s="101"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="31"/>
-      <c r="S33" s="26"/>
-      <c r="T33" s="23"/>
-      <c r="U33" s="26"/>
-      <c r="V33" s="26"/>
-    </row>
-    <row r="34" spans="1:39" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="33"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="101"/>
-      <c r="D34" s="101"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="51"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="31"/>
-      <c r="S34" s="26"/>
-      <c r="T34" s="23"/>
-      <c r="U34" s="26"/>
-      <c r="V34" s="26"/>
-    </row>
-    <row r="35" spans="1:39" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="33"/>
-      <c r="B35" s="55"/>
-      <c r="C35" s="102"/>
-      <c r="D35" s="102"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="51"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="3"/>
-      <c r="R35" s="31"/>
-      <c r="S35" s="26"/>
-      <c r="T35" s="23"/>
-      <c r="U35" s="26"/>
-      <c r="V35" s="26"/>
-    </row>
-    <row r="36" spans="1:39" ht="28.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="77" t="s">
+      <c r="R9" s="25"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="AI9"/>
+      <c r="AJ9"/>
+      <c r="AK9" s="118"/>
+      <c r="AL9" s="118"/>
+      <c r="AM9" s="118"/>
+      <c r="AN9" s="118"/>
+      <c r="AO9" s="118"/>
+      <c r="AP9" s="118"/>
+      <c r="AQ9" s="118"/>
+      <c r="AR9" s="118"/>
+      <c r="AS9" s="118"/>
+      <c r="AT9" s="118"/>
+      <c r="AU9" s="118"/>
+      <c r="AV9" s="118"/>
+      <c r="AW9" s="118"/>
+      <c r="AX9" s="118"/>
+    </row>
+    <row r="10" spans="1:50" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="27"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="64"/>
+      <c r="P10" s="65"/>
+      <c r="Q10" s="67"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="68"/>
+      <c r="T10" s="69"/>
+      <c r="U10" s="68"/>
+      <c r="V10" s="68"/>
+      <c r="AI10"/>
+      <c r="AJ10"/>
+      <c r="AK10" s="118"/>
+      <c r="AL10" s="118"/>
+      <c r="AM10" s="118"/>
+      <c r="AN10" s="118"/>
+      <c r="AO10" s="118"/>
+      <c r="AP10" s="118"/>
+      <c r="AQ10" s="118"/>
+      <c r="AR10" s="118"/>
+      <c r="AS10" s="118"/>
+      <c r="AT10" s="118"/>
+      <c r="AU10" s="118"/>
+      <c r="AV10" s="118"/>
+      <c r="AW10" s="118"/>
+      <c r="AX10" s="118"/>
+    </row>
+    <row r="11" spans="1:50" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A11" s="27"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="65"/>
+      <c r="Q11" s="67"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="68"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="68"/>
+      <c r="V11" s="68"/>
+      <c r="AJ11" s="47"/>
+      <c r="AK11" s="47"/>
+      <c r="AL11" s="118"/>
+      <c r="AM11" s="118"/>
+      <c r="AN11" s="118"/>
+      <c r="AO11" s="118"/>
+      <c r="AP11" s="118"/>
+      <c r="AQ11" s="118"/>
+      <c r="AR11" s="118"/>
+      <c r="AS11" s="118"/>
+      <c r="AT11" s="118"/>
+      <c r="AU11" s="118"/>
+      <c r="AV11" s="118"/>
+      <c r="AW11" s="118"/>
+    </row>
+    <row r="12" spans="1:50" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A12" s="27"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="67"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="68"/>
+      <c r="T12" s="69"/>
+      <c r="U12" s="68"/>
+      <c r="V12" s="68"/>
+      <c r="AJ12" s="48"/>
+      <c r="AK12" s="48"/>
+      <c r="AL12" s="118"/>
+      <c r="AM12" s="118"/>
+      <c r="AN12" s="118"/>
+      <c r="AO12" s="118"/>
+      <c r="AP12" s="118"/>
+      <c r="AQ12" s="118"/>
+      <c r="AR12" s="118"/>
+      <c r="AS12" s="118"/>
+      <c r="AT12" s="118"/>
+      <c r="AU12" s="118"/>
+      <c r="AV12" s="118"/>
+      <c r="AW12" s="118"/>
+    </row>
+    <row r="13" spans="1:50" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A13" s="27"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="64"/>
+      <c r="P13" s="65"/>
+      <c r="Q13" s="67"/>
+      <c r="R13" s="58"/>
+      <c r="S13" s="68"/>
+      <c r="T13" s="69"/>
+      <c r="U13" s="68"/>
+      <c r="V13" s="68"/>
+      <c r="AJ13" s="48"/>
+      <c r="AK13" s="48"/>
+      <c r="AL13" s="118"/>
+      <c r="AM13" s="118"/>
+      <c r="AN13" s="118"/>
+      <c r="AO13" s="118"/>
+      <c r="AP13" s="118"/>
+      <c r="AQ13" s="118"/>
+      <c r="AR13" s="118"/>
+      <c r="AS13" s="118"/>
+      <c r="AT13" s="118"/>
+      <c r="AU13" s="118"/>
+      <c r="AV13" s="118"/>
+      <c r="AW13" s="118"/>
+    </row>
+    <row r="14" spans="1:50" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="27"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="64"/>
+      <c r="O14" s="64"/>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="67"/>
+      <c r="R14" s="58"/>
+      <c r="S14" s="68"/>
+      <c r="T14" s="69"/>
+      <c r="U14" s="68"/>
+      <c r="V14" s="68"/>
+      <c r="AL14" s="118"/>
+      <c r="AM14" s="118"/>
+      <c r="AN14" s="118"/>
+      <c r="AO14" s="118"/>
+      <c r="AP14" s="118"/>
+      <c r="AQ14" s="118"/>
+      <c r="AR14" s="118"/>
+      <c r="AS14" s="118"/>
+      <c r="AT14" s="118"/>
+      <c r="AU14" s="118"/>
+      <c r="AV14" s="118"/>
+      <c r="AW14" s="118"/>
+    </row>
+    <row r="15" spans="1:50" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="27"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="64"/>
+      <c r="P15" s="65"/>
+      <c r="Q15" s="67"/>
+      <c r="R15" s="58"/>
+      <c r="S15" s="68"/>
+      <c r="T15" s="69"/>
+      <c r="U15" s="68"/>
+      <c r="V15" s="68"/>
+    </row>
+    <row r="16" spans="1:50" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="27"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="64"/>
+      <c r="O16" s="64"/>
+      <c r="P16" s="65"/>
+      <c r="Q16" s="67"/>
+      <c r="R16" s="58"/>
+      <c r="S16" s="68"/>
+      <c r="T16" s="69"/>
+      <c r="U16" s="68"/>
+      <c r="V16" s="68"/>
+    </row>
+    <row r="17" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="27"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="64"/>
+      <c r="P17" s="65"/>
+      <c r="Q17" s="67"/>
+      <c r="R17" s="58"/>
+      <c r="S17" s="68"/>
+      <c r="T17" s="69"/>
+      <c r="U17" s="68"/>
+      <c r="V17" s="68"/>
+    </row>
+    <row r="18" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="27"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="64"/>
+      <c r="O18" s="64"/>
+      <c r="P18" s="65"/>
+      <c r="Q18" s="67"/>
+      <c r="R18" s="58"/>
+      <c r="S18" s="68"/>
+      <c r="T18" s="69"/>
+      <c r="U18" s="68"/>
+      <c r="V18" s="68"/>
+    </row>
+    <row r="19" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="27"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="64"/>
+      <c r="P19" s="65"/>
+      <c r="Q19" s="67"/>
+      <c r="R19" s="58"/>
+      <c r="S19" s="68"/>
+      <c r="T19" s="69"/>
+      <c r="U19" s="68"/>
+      <c r="V19" s="68"/>
+    </row>
+    <row r="20" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="27"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="66"/>
+      <c r="N20" s="64"/>
+      <c r="O20" s="64"/>
+      <c r="P20" s="65"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="58"/>
+      <c r="S20" s="68"/>
+      <c r="T20" s="69"/>
+      <c r="U20" s="68"/>
+      <c r="V20" s="68"/>
+    </row>
+    <row r="21" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="27"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="66"/>
+      <c r="N21" s="64"/>
+      <c r="O21" s="64"/>
+      <c r="P21" s="65"/>
+      <c r="Q21" s="67"/>
+      <c r="R21" s="58"/>
+      <c r="S21" s="68"/>
+      <c r="T21" s="69"/>
+      <c r="U21" s="68"/>
+      <c r="V21" s="68"/>
+    </row>
+    <row r="22" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="27"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="65"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="64"/>
+      <c r="O22" s="64"/>
+      <c r="P22" s="65"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="58"/>
+      <c r="S22" s="68"/>
+      <c r="T22" s="69"/>
+      <c r="U22" s="68"/>
+      <c r="V22" s="68"/>
+    </row>
+    <row r="23" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="27"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="65"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="64"/>
+      <c r="P23" s="65"/>
+      <c r="Q23" s="67"/>
+      <c r="R23" s="58"/>
+      <c r="S23" s="68"/>
+      <c r="T23" s="69"/>
+      <c r="U23" s="68"/>
+      <c r="V23" s="68"/>
+    </row>
+    <row r="24" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="27"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="65"/>
+      <c r="M24" s="66"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="65"/>
+      <c r="Q24" s="67"/>
+      <c r="R24" s="58"/>
+      <c r="S24" s="68"/>
+      <c r="T24" s="68"/>
+      <c r="U24" s="68"/>
+      <c r="V24" s="68"/>
+    </row>
+    <row r="25" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="27"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="66"/>
+      <c r="N25" s="64"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="65"/>
+      <c r="Q25" s="67"/>
+      <c r="R25" s="58"/>
+      <c r="S25" s="68"/>
+      <c r="T25" s="69"/>
+      <c r="U25" s="68"/>
+      <c r="V25" s="68"/>
+    </row>
+    <row r="26" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="27"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="63"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="66"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="64"/>
+      <c r="P26" s="65"/>
+      <c r="Q26" s="67"/>
+      <c r="R26" s="58"/>
+      <c r="S26" s="68"/>
+      <c r="T26" s="69"/>
+      <c r="U26" s="68"/>
+      <c r="V26" s="68"/>
+    </row>
+    <row r="27" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="27"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="66"/>
+      <c r="N27" s="64"/>
+      <c r="O27" s="64"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="67"/>
+      <c r="R27" s="58"/>
+      <c r="S27" s="68"/>
+      <c r="T27" s="69"/>
+      <c r="U27" s="68"/>
+      <c r="V27" s="68"/>
+    </row>
+    <row r="28" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="27"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="66"/>
+      <c r="N28" s="64"/>
+      <c r="O28" s="64"/>
+      <c r="P28" s="65"/>
+      <c r="Q28" s="67"/>
+      <c r="R28" s="58"/>
+      <c r="S28" s="68"/>
+      <c r="T28" s="69"/>
+      <c r="U28" s="68"/>
+      <c r="V28" s="68"/>
+    </row>
+    <row r="29" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="27"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="65"/>
+      <c r="M29" s="66"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="64"/>
+      <c r="P29" s="65"/>
+      <c r="Q29" s="67"/>
+      <c r="R29" s="58"/>
+      <c r="S29" s="68"/>
+      <c r="T29" s="69"/>
+      <c r="U29" s="68"/>
+      <c r="V29" s="68"/>
+    </row>
+    <row r="30" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="27"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="65"/>
+      <c r="M30" s="66"/>
+      <c r="N30" s="64"/>
+      <c r="O30" s="64"/>
+      <c r="P30" s="65"/>
+      <c r="Q30" s="67"/>
+      <c r="R30" s="58"/>
+      <c r="S30" s="68"/>
+      <c r="T30" s="69"/>
+      <c r="U30" s="68"/>
+      <c r="V30" s="68"/>
+    </row>
+    <row r="31" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="27"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="65"/>
+      <c r="M31" s="66"/>
+      <c r="N31" s="64"/>
+      <c r="O31" s="64"/>
+      <c r="P31" s="65"/>
+      <c r="Q31" s="67"/>
+      <c r="R31" s="58"/>
+      <c r="S31" s="68"/>
+      <c r="T31" s="69"/>
+      <c r="U31" s="68"/>
+      <c r="V31" s="68"/>
+    </row>
+    <row r="32" spans="1:22" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="27"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="66"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="65"/>
+      <c r="Q32" s="67"/>
+      <c r="R32" s="58"/>
+      <c r="S32" s="68"/>
+      <c r="T32" s="69"/>
+      <c r="U32" s="68"/>
+      <c r="V32" s="68"/>
+    </row>
+    <row r="33" spans="1:39" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="27"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="64"/>
+      <c r="L33" s="65"/>
+      <c r="M33" s="66"/>
+      <c r="N33" s="64"/>
+      <c r="O33" s="64"/>
+      <c r="P33" s="65"/>
+      <c r="Q33" s="67"/>
+      <c r="R33" s="58"/>
+      <c r="S33" s="68"/>
+      <c r="T33" s="69"/>
+      <c r="U33" s="68"/>
+      <c r="V33" s="68"/>
+    </row>
+    <row r="34" spans="1:39" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="27"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="63"/>
+      <c r="K34" s="64"/>
+      <c r="L34" s="65"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="64"/>
+      <c r="O34" s="64"/>
+      <c r="P34" s="65"/>
+      <c r="Q34" s="67"/>
+      <c r="R34" s="58"/>
+      <c r="S34" s="68"/>
+      <c r="T34" s="69"/>
+      <c r="U34" s="68"/>
+      <c r="V34" s="68"/>
+    </row>
+    <row r="35" spans="1:39" s="4" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="27"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="63"/>
+      <c r="K35" s="64"/>
+      <c r="L35" s="65"/>
+      <c r="M35" s="66"/>
+      <c r="N35" s="64"/>
+      <c r="O35" s="64"/>
+      <c r="P35" s="65"/>
+      <c r="Q35" s="67"/>
+      <c r="R35" s="58"/>
+      <c r="S35" s="68"/>
+      <c r="T35" s="69"/>
+      <c r="U35" s="68"/>
+      <c r="V35" s="68"/>
+    </row>
+    <row r="36" spans="1:39" ht="28.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="78"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="72">
+      <c r="B36" s="98"/>
+      <c r="C36" s="98"/>
+      <c r="D36" s="92">
         <f>H36+J36+K36+L36+M36+N36+O36+P36+S36+T36+U36+V36</f>
         <v>0</v>
       </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="20">
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="72">
         <f>SUM(H5:H35)</f>
         <v>0</v>
       </c>
-      <c r="I36" s="21"/>
-      <c r="J36" s="22">
+      <c r="I36" s="73"/>
+      <c r="J36" s="74">
         <f t="shared" ref="J36:V36" si="0">SUM(J5:J35)</f>
         <v>0</v>
       </c>
-      <c r="K36" s="22">
+      <c r="K36" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L36" s="22">
+      <c r="L36" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M36" s="22">
+      <c r="M36" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N36" s="22">
+      <c r="N36" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O36" s="22">
+      <c r="O36" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P36" s="22">
+      <c r="P36" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q36" s="22">
+      <c r="Q36" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R36" s="22">
+      <c r="R36" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S36" s="24">
+      <c r="S36" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T36" s="24">
+      <c r="T36" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U36" s="24">
+      <c r="U36" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V36" s="24">
+      <c r="V36" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2757,54 +2832,59 @@
       <c r="AM36" s="5"/>
     </row>
     <row r="37" spans="1:39" ht="19.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="58" t="s">
+      <c r="A37" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="59"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="73"/>
-      <c r="H37" s="16" t="s">
+      <c r="B37" s="79"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="93"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I37" s="56"/>
-      <c r="J37" s="18" t="s">
+      <c r="I37" s="76"/>
+      <c r="J37" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="K37" s="18" t="s">
+      <c r="K37" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="L37" s="18" t="s">
+      <c r="L37" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="M37" s="18" t="s">
+      <c r="M37" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="N37" s="18" t="s">
+      <c r="N37" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="O37" s="18" t="s">
+      <c r="O37" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="P37" s="18" t="s">
+      <c r="P37" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="R37"/>
-      <c r="S37" s="27" t="s">
+      <c r="Q37" s="77"/>
+      <c r="R37" s="77"/>
+      <c r="S37" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="T37" s="27" t="s">
+      <c r="T37" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="U37" s="27" t="s">
+      <c r="U37" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="V37" s="27" t="s">
+      <c r="V37" s="21" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="AI1:AV10"/>
+    <mergeCell ref="AK1:AX10"/>
+    <mergeCell ref="AL11:AW14"/>
     <mergeCell ref="S2:S4"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="B2:B4"/>
@@ -2818,7 +2898,6 @@
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="Q2:R3"/>
     <mergeCell ref="M3:M4"/>
-    <mergeCell ref="AL11:AS14"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="U2:U4"/>
@@ -2835,12 +2914,14 @@
     <mergeCell ref="T2:T4"/>
     <mergeCell ref="C2:C4"/>
   </mergeCells>
+  <phoneticPr fontId="23" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="B6:B36" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"X"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="81" fitToWidth="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" scale="93" fitToWidth="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>